<commit_message>
commiting all test cases
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vempv\Desktop\zaaaagain\DISFramework (1)\DISFramework\DISFramework\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB2811D-A91E-4B44-B7F4-CE67E2DCE25F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C40370BB-C712-4CE4-9B68-055CE7CA1CB2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19460" windowHeight="11060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +25,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Activity!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="C32:F38"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="424">
   <si>
     <t>Environment</t>
   </si>
@@ -811,9 +807,6 @@
   </si>
   <si>
     <t>DR.4.2-2</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>ValidateIndicatorDetails</t>
@@ -1738,7 +1731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1805,7 +1798,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1814,7 +1807,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G2">
         <v>15</v>
@@ -1829,7 +1822,7 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1895,7 +1888,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
@@ -1955,10 +1948,10 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>239</v>
@@ -1975,7 +1968,7 @@
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>47</v>
@@ -1987,42 +1980,42 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2080,13 +2073,13 @@
         <v>217</v>
       </c>
       <c r="K1" t="s">
+        <v>363</v>
+      </c>
+      <c r="L1" t="s">
         <v>364</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>365</v>
-      </c>
-      <c r="M1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -2097,7 +2090,7 @@
         <v>170</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>172</v>
@@ -2123,7 +2116,7 @@
         <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
         <v>195</v>
@@ -2143,7 +2136,7 @@
         <v>198</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
         <v>197</v>
@@ -2166,7 +2159,7 @@
         <v>214</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D5" t="s">
         <v>215</v>
@@ -2183,31 +2176,31 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D6" t="s">
+        <v>361</v>
+      </c>
+      <c r="E6" t="s">
         <v>362</v>
       </c>
-      <c r="E6" t="s">
-        <v>363</v>
-      </c>
       <c r="J6" t="s">
+        <v>366</v>
+      </c>
+      <c r="K6" t="s">
         <v>367</v>
       </c>
-      <c r="K6" t="s">
-        <v>368</v>
-      </c>
       <c r="L6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2264,7 @@
         <v>210</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>211</v>
@@ -2304,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="C32" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2400,7 +2393,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
@@ -2417,19 +2410,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" t="s">
         <v>289</v>
       </c>
-      <c r="C4" t="s">
-        <v>290</v>
-      </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -2446,19 +2439,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -2487,7 +2480,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
@@ -2516,7 +2509,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -2533,19 +2526,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -2562,19 +2555,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -2603,7 +2596,7 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
@@ -2632,7 +2625,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -2649,19 +2642,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>335</v>
+      </c>
+      <c r="C12" t="s">
         <v>336</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>337</v>
-      </c>
-      <c r="D12" t="s">
-        <v>338</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -2678,19 +2671,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C13" t="s">
         <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
@@ -2707,19 +2700,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" t="s">
+        <v>309</v>
+      </c>
+      <c r="D14" t="s">
         <v>308</v>
-      </c>
-      <c r="C14" t="s">
-        <v>310</v>
-      </c>
-      <c r="D14" t="s">
-        <v>309</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -2736,19 +2729,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C15" t="s">
+        <v>312</v>
+      </c>
+      <c r="D15" t="s">
         <v>311</v>
-      </c>
-      <c r="C15" t="s">
-        <v>313</v>
-      </c>
-      <c r="D15" t="s">
-        <v>312</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -2765,19 +2758,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C16" t="s">
         <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
@@ -2794,19 +2787,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -2823,19 +2816,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>319</v>
+      </c>
+      <c r="C18" t="s">
         <v>320</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>321</v>
-      </c>
-      <c r="D18" t="s">
-        <v>322</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
@@ -2852,7 +2845,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C19" t="s">
         <v>114</v>
@@ -2864,7 +2857,7 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>
@@ -2881,19 +2874,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C20" t="s">
+        <v>368</v>
+      </c>
+      <c r="D20" t="s">
         <v>369</v>
-      </c>
-      <c r="D20" t="s">
-        <v>370</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
@@ -2910,19 +2903,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>374</v>
+      </c>
+      <c r="C21" t="s">
+        <v>368</v>
+      </c>
+      <c r="D21" t="s">
         <v>375</v>
-      </c>
-      <c r="C21" t="s">
-        <v>369</v>
-      </c>
-      <c r="D21" t="s">
-        <v>376</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G21" t="s">
         <v>24</v>
@@ -2939,19 +2932,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
@@ -2980,7 +2973,7 @@
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
@@ -3009,7 +3002,7 @@
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
@@ -3038,7 +3031,7 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
         <v>24</v>
@@ -3067,7 +3060,7 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G26" t="s">
         <v>24</v>
@@ -3084,19 +3077,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C27" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" t="s">
         <v>258</v>
-      </c>
-      <c r="C27" t="s">
-        <v>269</v>
-      </c>
-      <c r="D27" t="s">
-        <v>259</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
@@ -3113,19 +3106,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C28" t="s">
         <v>181</v>
       </c>
       <c r="D28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G28" t="s">
         <v>24</v>
@@ -3142,19 +3135,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C29" t="s">
         <v>191</v>
       </c>
       <c r="D29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E29" t="s">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
@@ -3171,19 +3164,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C30" t="s">
         <v>181</v>
       </c>
       <c r="D30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
@@ -3200,7 +3193,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C31" t="s">
         <v>181</v>
@@ -3212,7 +3205,7 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G31" t="s">
         <v>24</v>
@@ -3229,19 +3222,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -3258,19 +3251,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>414</v>
+      </c>
+      <c r="C33" t="s">
         <v>415</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>416</v>
-      </c>
-      <c r="D33" t="s">
-        <v>417</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G33" t="s">
         <v>24</v>
@@ -3299,7 +3292,7 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G34" t="s">
         <v>24</v>
@@ -3328,7 +3321,7 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
@@ -3357,7 +3350,7 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G36" t="s">
         <v>24</v>
@@ -3374,19 +3367,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>359</v>
+      </c>
+      <c r="C37" t="s">
         <v>360</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>361</v>
-      </c>
-      <c r="D37" t="s">
-        <v>362</v>
       </c>
       <c r="E37" t="s">
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G37" t="s">
         <v>24</v>
@@ -3415,7 +3408,7 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G38" t="s">
         <v>24</v>
@@ -3444,7 +3437,7 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
@@ -3473,7 +3466,7 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G40" t="s">
         <v>24</v>
@@ -3502,7 +3495,7 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G41" t="s">
         <v>24</v>
@@ -3531,7 +3524,7 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="H42" t="s">
         <v>238</v>
@@ -3545,28 +3538,28 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>390</v>
+      </c>
+      <c r="C43" t="s">
         <v>391</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>392</v>
-      </c>
-      <c r="D43" t="s">
-        <v>393</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G43" t="s">
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I43" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -3574,28 +3567,28 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>400</v>
+      </c>
+      <c r="C44" t="s">
+        <v>402</v>
+      </c>
+      <c r="D44" t="s">
         <v>401</v>
-      </c>
-      <c r="C44" t="s">
-        <v>403</v>
-      </c>
-      <c r="D44" t="s">
-        <v>402</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G44" t="s">
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3603,28 +3596,28 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>406</v>
+      </c>
+      <c r="C45" t="s">
         <v>407</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>408</v>
-      </c>
-      <c r="D45" t="s">
-        <v>409</v>
       </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="G45" t="s">
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I45" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -3672,112 +3665,112 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>196</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="J1" t="s">
         <v>389</v>
       </c>
-      <c r="J1" t="s">
-        <v>390</v>
-      </c>
       <c r="K1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L1" t="s">
+        <v>404</v>
+      </c>
+      <c r="M1" t="s">
+        <v>403</v>
+      </c>
+      <c r="N1" t="s">
         <v>405</v>
-      </c>
-      <c r="M1" t="s">
-        <v>404</v>
-      </c>
-      <c r="N1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
       </c>
       <c r="I2" t="s">
+        <v>395</v>
+      </c>
+      <c r="J2" t="s">
         <v>396</v>
       </c>
-      <c r="J2" t="s">
-        <v>397</v>
-      </c>
       <c r="K2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" t="s">
         <v>401</v>
       </c>
-      <c r="B3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D3" t="s">
-        <v>402</v>
-      </c>
       <c r="K3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
+        <v>408</v>
+      </c>
+      <c r="F4" t="s">
         <v>409</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>410</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" t="s">
+        <v>413</v>
+      </c>
+      <c r="M4" t="s">
         <v>412</v>
-      </c>
-      <c r="L4" t="s">
-        <v>414</v>
-      </c>
-      <c r="M4" t="s">
-        <v>413</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -3847,7 +3840,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F1" t="s">
         <v>73</v>
@@ -3940,49 +3933,49 @@
         <v>125</v>
       </c>
       <c r="AJ1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AK1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AL1" t="s">
         <v>314</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>315</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>316</v>
       </c>
-      <c r="AN1" t="s">
-        <v>317</v>
-      </c>
       <c r="AO1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AP1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>340</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>341</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>342</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>343</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>344</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>345</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>346</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>347</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.35">
@@ -3993,7 +3986,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -4055,7 +4048,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
         <v>109</v>
@@ -4136,7 +4129,7 @@
         <v>119</v>
       </c>
       <c r="AE3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AF3" t="s">
         <v>235</v>
@@ -4153,19 +4146,19 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G4" t="s">
         <v>89</v>
@@ -4213,7 +4206,7 @@
         <v>98</v>
       </c>
       <c r="V4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="W4">
         <v>234</v>
@@ -4240,7 +4233,7 @@
         <v>119</v>
       </c>
       <c r="AE4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AF4" t="s">
         <v>235</v>
@@ -4257,53 +4250,53 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" t="s">
         <v>308</v>
       </c>
-      <c r="B5" t="s">
-        <v>307</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D5" t="s">
-        <v>309</v>
-      </c>
       <c r="AJ5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" t="s">
         <v>311</v>
       </c>
-      <c r="B6" t="s">
-        <v>307</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D6" t="s">
-        <v>312</v>
-      </c>
       <c r="AJ6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D7" t="s">
+        <v>322</v>
+      </c>
+      <c r="F7" t="s">
         <v>323</v>
-      </c>
-      <c r="F7" t="s">
-        <v>324</v>
       </c>
       <c r="G7" t="s">
         <v>89</v>
@@ -4312,7 +4305,7 @@
         <v>90</v>
       </c>
       <c r="I7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J7" t="s">
         <v>63</v>
@@ -4333,10 +4326,10 @@
         <v>255</v>
       </c>
       <c r="P7" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="R7" t="s">
         <v>97</v>
@@ -4351,7 +4344,7 @@
         <v>98</v>
       </c>
       <c r="V7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="W7">
         <v>234</v>
@@ -4378,7 +4371,7 @@
         <v>119</v>
       </c>
       <c r="AE7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AF7" t="s">
         <v>235</v>
@@ -4395,36 +4388,36 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AJ8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AJ9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AK9">
         <v>23.33</v>
@@ -4436,71 +4429,71 @@
         <v>2018</v>
       </c>
       <c r="AN9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F10" t="s">
         <v>338</v>
       </c>
-      <c r="F10" t="s">
-        <v>339</v>
-      </c>
       <c r="AO10" t="s">
+        <v>354</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>348</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>349</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>350</v>
+      </c>
+      <c r="AT10" t="s">
         <v>355</v>
       </c>
-      <c r="AP10" t="s">
-        <v>349</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>350</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>354</v>
-      </c>
-      <c r="AS10" t="s">
+      <c r="AU10" t="s">
         <v>351</v>
       </c>
-      <c r="AT10" t="s">
+      <c r="AV10" t="s">
         <v>356</v>
       </c>
-      <c r="AU10" t="s">
-        <v>352</v>
-      </c>
-      <c r="AV10" t="s">
+      <c r="AW10" t="s">
         <v>357</v>
       </c>
-      <c r="AW10" t="s">
+      <c r="AX10" t="s">
         <v>358</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D11" t="s">
+        <v>372</v>
+      </c>
+      <c r="F11" t="s">
         <v>373</v>
-      </c>
-      <c r="F11" t="s">
-        <v>374</v>
       </c>
       <c r="G11" t="s">
         <v>89</v>
@@ -4575,7 +4568,7 @@
         <v>119</v>
       </c>
       <c r="AE11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AF11" t="s">
         <v>235</v>
@@ -4592,71 +4585,71 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>371</v>
+      </c>
+      <c r="B12" t="s">
+        <v>370</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D12" t="s">
         <v>372</v>
       </c>
-      <c r="B12" t="s">
-        <v>371</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>377</v>
+      </c>
+      <c r="F12" t="s">
         <v>373</v>
-      </c>
-      <c r="E12" t="s">
-        <v>378</v>
-      </c>
-      <c r="F12" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>374</v>
+      </c>
+      <c r="B13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D13" t="s">
         <v>375</v>
       </c>
-      <c r="B13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>376</v>
-      </c>
-      <c r="E13" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>381</v>
+      </c>
+      <c r="B14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D14" t="s">
+        <v>380</v>
+      </c>
+      <c r="F14" t="s">
         <v>382</v>
       </c>
-      <c r="B14" t="s">
-        <v>382</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D14" t="s">
-        <v>381</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="AJ14" t="s">
         <v>383</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>384</v>
       </c>
       <c r="AK14">
         <v>345</v>
       </c>
       <c r="AL14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AM14">
         <v>2020</v>
       </c>
       <c r="AN14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -4704,7 +4697,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F1" t="s">
         <v>54</v>
@@ -4734,7 +4727,7 @@
         <v>62</v>
       </c>
       <c r="O1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -4745,7 +4738,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -4780,19 +4773,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F3" t="s">
         <v>298</v>
-      </c>
-      <c r="F3" t="s">
-        <v>299</v>
       </c>
       <c r="G3" t="s">
         <v>120</v>
@@ -4813,7 +4806,7 @@
         <v>253</v>
       </c>
       <c r="M3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N3" t="s">
         <v>66</v>
@@ -4821,19 +4814,19 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" t="s">
         <v>301</v>
       </c>
-      <c r="B4" t="s">
-        <v>302</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4914,10 +4907,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="E2" t="s">
         <v>237</v>
@@ -5015,7 +5008,7 @@
         <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G1" t="s">
         <v>127</v>
@@ -5084,19 +5077,19 @@
         <v>187</v>
       </c>
       <c r="AC1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AD1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AE1" t="s">
         <v>262</v>
       </c>
-      <c r="AE1" t="s">
-        <v>263</v>
-      </c>
       <c r="AF1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AG1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
@@ -5107,7 +5100,7 @@
         <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>146</v>
@@ -5178,7 +5171,7 @@
         <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
         <v>183</v>
@@ -5207,7 +5200,7 @@
         <v>180</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
         <v>184</v>
@@ -5233,7 +5226,7 @@
         <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D5" t="s">
         <v>184</v>
@@ -5242,7 +5235,7 @@
         <v>185</v>
       </c>
       <c r="F5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G5" t="s">
         <v>63</v>
@@ -5256,22 +5249,22 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" t="s">
         <v>258</v>
       </c>
-      <c r="B6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D6" t="s">
-        <v>259</v>
-      </c>
       <c r="E6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K6" t="s">
         <v>154</v>
@@ -5280,33 +5273,33 @@
         <v>158</v>
       </c>
       <c r="AC6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AD6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AE6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7" t="s">
         <v>275</v>
-      </c>
-      <c r="E7" t="s">
-        <v>276</v>
       </c>
       <c r="K7" t="s">
         <v>154</v>
@@ -5315,79 +5308,79 @@
         <v>188</v>
       </c>
       <c r="AB7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D8" t="s">
         <v>274</v>
       </c>
-      <c r="B8" t="s">
-        <v>273</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>275</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>276</v>
       </c>
-      <c r="F8" t="s">
-        <v>277</v>
-      </c>
       <c r="K8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AA8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" t="s">
         <v>281</v>
       </c>
-      <c r="B9" t="s">
-        <v>281</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>282</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>283</v>
       </c>
-      <c r="F9" t="s">
+      <c r="K9" t="s">
+        <v>279</v>
+      </c>
+      <c r="AA9" t="s">
         <v>284</v>
       </c>
-      <c r="K9" t="s">
-        <v>280</v>
-      </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>285</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D10" t="s">
         <v>182</v>
       </c>
       <c r="E10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K10" t="s">
         <v>154</v>
@@ -5401,39 +5394,39 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
       </c>
       <c r="AG12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -5479,7 +5472,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -5493,7 +5486,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
         <v>102</v>
@@ -5553,7 +5546,7 @@
         <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -5570,7 +5563,7 @@
         <v>224</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
         <v>223</v>
@@ -5587,7 +5580,7 @@
         <v>226</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
         <v>227</v>
@@ -5604,7 +5597,7 @@
         <v>229</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D5" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
updated few testcases to yes
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C40370BB-C712-4CE4-9B68-055CE7CA1CB2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C708299-D404-4A55-B154-8634550C7CA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="19460" windowHeight="11060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Activity!$A$1:$U$2</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="C32:F38"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="425">
   <si>
     <t>Environment</t>
   </si>
@@ -1308,6 +1312,9 @@
   </si>
   <si>
     <t>.\\POMFramework\\Reports\\</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -2297,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F45"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3060,7 +3067,7 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G26" t="s">
         <v>24</v>
@@ -3089,7 +3096,7 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
@@ -3118,7 +3125,7 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G28" t="s">
         <v>24</v>
@@ -3147,7 +3154,7 @@
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
@@ -3176,7 +3183,7 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
@@ -3205,7 +3212,7 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G31" t="s">
         <v>24</v>
@@ -3234,7 +3241,7 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -3263,7 +3270,7 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G33" t="s">
         <v>24</v>
@@ -3292,7 +3299,7 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G34" t="s">
         <v>24</v>
@@ -3321,7 +3328,7 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
@@ -3350,7 +3357,7 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G36" t="s">
         <v>24</v>
@@ -3379,7 +3386,7 @@
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G37" t="s">
         <v>24</v>
@@ -3408,7 +3415,7 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G38" t="s">
         <v>24</v>
@@ -3437,7 +3444,7 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
@@ -3466,7 +3473,7 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G40" t="s">
         <v>24</v>
@@ -3495,7 +3502,7 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G41" t="s">
         <v>24</v>
@@ -3524,7 +3531,7 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="H42" t="s">
         <v>238</v>
@@ -3550,7 +3557,7 @@
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G43" t="s">
         <v>24</v>
@@ -3579,7 +3586,7 @@
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G44" t="s">
         <v>24</v>
@@ -3608,7 +3615,7 @@
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="G45" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Marking first three testcases as yes.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vempv\git\LatestDis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vamsi Vempati\git\SantoshLatestZahid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97FD1F3-BE9E-4E51-A92D-EE262BA8A302}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4645339-CB55-4255-91AA-F405AE6EFF53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1738,28 +1738,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="66" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1800,7 +1798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1852,16 +1850,16 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1887,7 +1885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1913,7 +1911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
     </row>
   </sheetData>
@@ -1929,19 +1927,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1967,7 +1965,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1985,7 +1983,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -2005,7 +2003,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>290</v>
       </c>
@@ -2038,17 +2036,17 @@
       <selection activeCell="C6" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2089,7 +2087,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -2115,7 +2113,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -2135,7 +2133,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -2158,7 +2156,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -2181,7 +2179,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>359</v>
       </c>
@@ -2224,14 +2222,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2263,7 +2261,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -2305,24 +2303,24 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -2354,7 +2352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2383,7 +2381,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2412,7 +2410,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2429,7 +2427,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>424</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -2441,7 +2439,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2470,7 +2468,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2499,7 +2497,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2528,7 +2526,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2557,7 +2555,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2586,7 +2584,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2615,7 +2613,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2644,7 +2642,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2673,7 +2671,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2702,7 +2700,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2731,7 +2729,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2760,7 +2758,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2789,7 +2787,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2818,7 +2816,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2847,7 +2845,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2905,7 +2903,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2934,7 +2932,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2963,7 +2961,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2992,7 +2990,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3021,7 +3019,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3050,7 +3048,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3079,7 +3077,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3108,7 +3106,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3137,7 +3135,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3166,7 +3164,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3195,7 +3193,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3224,7 +3222,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3253,7 +3251,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3282,7 +3280,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3311,7 +3309,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3340,7 +3338,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3369,7 +3367,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3398,7 +3396,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3427,7 +3425,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3456,7 +3454,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3485,7 +3483,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3514,7 +3512,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3540,7 +3538,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3569,7 +3567,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3598,7 +3596,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3641,24 +3639,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3702,7 +3700,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>390</v>
       </c>
@@ -3734,7 +3732,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>400</v>
       </c>
@@ -3751,7 +3749,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>406</v>
       </c>
@@ -3800,40 +3798,40 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7265625" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.1796875" customWidth="1"/>
-    <col min="42" max="42" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.140625" customWidth="1"/>
+    <col min="42" max="42" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3985,7 +3983,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -4047,7 +4045,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4151,7 +4149,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>306</v>
       </c>
@@ -4255,7 +4253,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>307</v>
       </c>
@@ -4272,7 +4270,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>310</v>
       </c>
@@ -4289,7 +4287,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>317</v>
       </c>
@@ -4393,7 +4391,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>318</v>
       </c>
@@ -4410,7 +4408,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>319</v>
       </c>
@@ -4439,7 +4437,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>335</v>
       </c>
@@ -4486,7 +4484,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>370</v>
       </c>
@@ -4590,7 +4588,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>371</v>
       </c>
@@ -4610,7 +4608,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>374</v>
       </c>
@@ -4627,7 +4625,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>381</v>
       </c>
@@ -4681,16 +4679,16 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
-    <col min="13" max="13" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4737,7 +4735,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -4778,7 +4776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>301</v>
       </c>
@@ -4819,7 +4817,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -4849,23 +4847,23 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.54296875" customWidth="1"/>
-    <col min="5" max="5" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4906,7 +4904,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -4947,7 +4945,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
@@ -4968,37 +4966,37 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -5099,7 +5097,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -5170,7 +5168,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -5199,7 +5197,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -5225,7 +5223,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -5254,7 +5252,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>257</v>
       </c>
@@ -5292,7 +5290,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -5318,7 +5316,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>273</v>
       </c>
@@ -5344,7 +5342,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -5373,7 +5371,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>332</v>
       </c>
@@ -5399,7 +5397,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>331</v>
       </c>
@@ -5416,7 +5414,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>414</v>
       </c>
@@ -5450,14 +5448,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" customWidth="1"/>
-    <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -5471,7 +5469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -5485,7 +5483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -5499,7 +5497,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
   </sheetData>
@@ -5516,16 +5514,16 @@
       <selection activeCell="C5" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -5545,7 +5543,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -5562,7 +5560,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>224</v>
       </c>
@@ -5579,7 +5577,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -5596,7 +5594,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Changed Code Added RunReport and other fields Added few dropdowns and text fields
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vamsi Vempati\git\SantoshLatestZahid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4645339-CB55-4255-91AA-F405AE6EFF53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF16843-848F-473D-B7F1-09DABAC2C669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="430">
   <si>
     <t>Environment</t>
   </si>
@@ -804,9 +804,6 @@
     <t>Hussin, Zahid</t>
   </si>
   <si>
-    <t>Health Office</t>
-  </si>
-  <si>
     <t>Hussin, Zahid (hussinzahid@gmail.com)</t>
   </si>
   <si>
@@ -1101,21 +1098,12 @@
     <t>DistribtionCode</t>
   </si>
   <si>
-    <t xml:space="preserve">Democracy &amp; Governance </t>
-  </si>
-  <si>
     <t>123-M</t>
   </si>
   <si>
     <t>CS-X12</t>
   </si>
   <si>
-    <t>DR.2 - Good Governance</t>
-  </si>
-  <si>
-    <t>DR.2.2 - Non-security Executive Authority - Function and Processes</t>
-  </si>
-  <si>
     <t>Unilateral</t>
   </si>
   <si>
@@ -1315,13 +1303,40 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Dhaka110045</t>
+  </si>
+  <si>
+    <t>MccM1141</t>
+  </si>
+  <si>
+    <t>Disable office</t>
+  </si>
+  <si>
+    <t>Hussin, Zahid (usaidtest3@gmail.com)</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Activity glaas 10/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable office </t>
+  </si>
+  <si>
+    <t>Rule of Law (ROL)</t>
+  </si>
+  <si>
+    <t>Culture of Lawfulness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1343,6 +1358,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1390,13 +1411,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1738,7 +1760,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1803,7 +1827,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1812,7 +1836,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G2">
         <v>15</v>
@@ -1827,7 +1851,7 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1893,7 +1917,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
@@ -1953,10 +1977,10 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>239</v>
@@ -1973,7 +1997,7 @@
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>47</v>
@@ -1985,42 +2009,42 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2078,13 +2102,13 @@
         <v>217</v>
       </c>
       <c r="K1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="L1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="M1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2095,7 +2119,7 @@
         <v>170</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>172</v>
@@ -2121,7 +2145,7 @@
         <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
         <v>195</v>
@@ -2141,7 +2165,7 @@
         <v>198</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D4" t="s">
         <v>197</v>
@@ -2164,7 +2188,7 @@
         <v>214</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D5" t="s">
         <v>215</v>
@@ -2181,31 +2205,31 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D6" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E6" t="s">
+        <v>358</v>
+      </c>
+      <c r="J6" t="s">
         <v>362</v>
       </c>
-      <c r="J6" t="s">
-        <v>366</v>
-      </c>
       <c r="K6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="L6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="M6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2269,7 +2293,7 @@
         <v>210</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>211</v>
@@ -2302,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,7 +2393,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>420</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -2398,7 +2422,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>420</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
@@ -2415,19 +2439,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4" t="s">
         <v>288</v>
       </c>
-      <c r="C4" t="s">
-        <v>289</v>
-      </c>
       <c r="D4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>420</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -2444,19 +2468,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -2485,7 +2509,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
@@ -2514,7 +2538,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -2531,19 +2555,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -2560,19 +2584,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -2601,7 +2625,7 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
@@ -2630,7 +2654,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -2647,19 +2671,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C12" t="s">
         <v>335</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>336</v>
-      </c>
-      <c r="D12" t="s">
-        <v>337</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -2676,19 +2700,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C13" t="s">
         <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
@@ -2705,19 +2729,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" t="s">
+        <v>308</v>
+      </c>
+      <c r="D14" t="s">
         <v>307</v>
-      </c>
-      <c r="C14" t="s">
-        <v>309</v>
-      </c>
-      <c r="D14" t="s">
-        <v>308</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -2734,19 +2758,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
         <v>310</v>
-      </c>
-      <c r="C15" t="s">
-        <v>312</v>
-      </c>
-      <c r="D15" t="s">
-        <v>311</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -2763,19 +2787,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C16" t="s">
         <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
@@ -2792,19 +2816,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -2821,19 +2845,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>318</v>
+      </c>
+      <c r="C18" t="s">
         <v>319</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>320</v>
-      </c>
-      <c r="D18" t="s">
-        <v>321</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
@@ -2850,7 +2874,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C19" t="s">
         <v>114</v>
@@ -2862,7 +2886,7 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>
@@ -2879,19 +2903,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C20" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D20" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
@@ -2908,19 +2932,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C21" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D21" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G21" t="s">
         <v>24</v>
@@ -2937,19 +2961,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D22" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
@@ -2978,7 +3002,7 @@
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
@@ -3007,7 +3031,7 @@
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
@@ -3036,7 +3060,7 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G25" t="s">
         <v>24</v>
@@ -3065,7 +3089,7 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G26" t="s">
         <v>24</v>
@@ -3082,19 +3106,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>256</v>
+      </c>
+      <c r="C27" t="s">
+        <v>267</v>
+      </c>
+      <c r="D27" t="s">
         <v>257</v>
-      </c>
-      <c r="C27" t="s">
-        <v>268</v>
-      </c>
-      <c r="D27" t="s">
-        <v>258</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
@@ -3111,19 +3135,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C28" t="s">
         <v>181</v>
       </c>
       <c r="D28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G28" t="s">
         <v>24</v>
@@ -3140,19 +3164,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C29" t="s">
         <v>191</v>
       </c>
       <c r="D29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E29" t="s">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
@@ -3169,19 +3193,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C30" t="s">
         <v>181</v>
       </c>
       <c r="D30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
@@ -3198,7 +3222,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C31" t="s">
         <v>181</v>
@@ -3210,7 +3234,7 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G31" t="s">
         <v>24</v>
@@ -3227,19 +3251,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -3256,19 +3280,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C33" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D33" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G33" t="s">
         <v>24</v>
@@ -3297,7 +3321,7 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G34" t="s">
         <v>24</v>
@@ -3326,7 +3350,7 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
@@ -3355,7 +3379,7 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G36" t="s">
         <v>24</v>
@@ -3372,19 +3396,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C37" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D37" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E37" t="s">
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G37" t="s">
         <v>24</v>
@@ -3413,7 +3437,7 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G38" t="s">
         <v>24</v>
@@ -3442,7 +3466,7 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
@@ -3471,7 +3495,7 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G40" t="s">
         <v>24</v>
@@ -3500,7 +3524,7 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G41" t="s">
         <v>24</v>
@@ -3529,7 +3553,7 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="H42" t="s">
         <v>238</v>
@@ -3543,28 +3567,28 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C43" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D43" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G43" t="s">
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I43" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3572,28 +3596,28 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C44" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D44" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G44" t="s">
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I44" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3601,28 +3625,28 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C45" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D45" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G45" t="s">
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I45" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -3670,112 +3694,112 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>196</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="J1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="K1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="L1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="M1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="N1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2" t="s">
         <v>390</v>
-      </c>
-      <c r="B2" t="s">
-        <v>390</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D2" t="s">
-        <v>392</v>
-      </c>
-      <c r="F2" t="s">
-        <v>397</v>
-      </c>
-      <c r="G2" t="s">
-        <v>394</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
       </c>
       <c r="I2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J2" t="s">
+        <v>392</v>
+      </c>
+      <c r="K2" t="s">
         <v>395</v>
-      </c>
-      <c r="J2" t="s">
-        <v>396</v>
-      </c>
-      <c r="K2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="K3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D4" t="s">
+        <v>404</v>
+      </c>
+      <c r="F4" t="s">
+        <v>405</v>
+      </c>
+      <c r="G4" t="s">
         <v>406</v>
       </c>
-      <c r="B4" t="s">
-        <v>406</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="I4" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="L4" t="s">
+        <v>409</v>
+      </c>
+      <c r="M4" t="s">
         <v>408</v>
-      </c>
-      <c r="F4" t="s">
-        <v>409</v>
-      </c>
-      <c r="G4" t="s">
-        <v>410</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="L4" t="s">
-        <v>413</v>
-      </c>
-      <c r="M4" t="s">
-        <v>412</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -3792,43 +3816,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AX14"/>
+  <dimension ref="A1:AX19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="AW10" sqref="AW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.140625" customWidth="1"/>
-    <col min="42" max="42" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -3845,7 +3888,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F1" t="s">
         <v>73</v>
@@ -3938,49 +3981,49 @@
         <v>125</v>
       </c>
       <c r="AJ1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AK1" t="s">
+        <v>312</v>
+      </c>
+      <c r="AL1" t="s">
         <v>313</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>314</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>315</v>
       </c>
-      <c r="AN1" t="s">
-        <v>316</v>
-      </c>
       <c r="AO1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AP1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>339</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>340</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>341</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>342</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>343</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>344</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>345</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>346</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
@@ -3991,7 +4034,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -4015,16 +4058,16 @@
         <v>93</v>
       </c>
       <c r="L2" t="s">
-        <v>254</v>
+        <v>423</v>
       </c>
       <c r="M2" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="N2" t="s">
         <v>94</v>
       </c>
       <c r="O2" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="P2" t="s">
         <v>95</v>
@@ -4039,7 +4082,7 @@
         <v>98765438</v>
       </c>
       <c r="T2">
-        <v>211</v>
+        <v>2113</v>
       </c>
       <c r="U2" t="s">
         <v>98</v>
@@ -4053,7 +4096,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
         <v>109</v>
@@ -4077,16 +4120,16 @@
         <v>93</v>
       </c>
       <c r="L3" t="s">
-        <v>120</v>
+        <v>423</v>
       </c>
       <c r="M3" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="N3" t="s">
         <v>94</v>
       </c>
       <c r="O3" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="P3" t="s">
         <v>95</v>
@@ -4125,7 +4168,7 @@
         <v>117</v>
       </c>
       <c r="AB3" t="s">
-        <v>233</v>
+        <v>424</v>
       </c>
       <c r="AC3">
         <v>45</v>
@@ -4134,7 +4177,7 @@
         <v>119</v>
       </c>
       <c r="AE3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="AF3" t="s">
         <v>235</v>
@@ -4151,19 +4194,19 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G4" t="s">
         <v>89</v>
@@ -4181,16 +4224,16 @@
         <v>93</v>
       </c>
       <c r="L4" t="s">
-        <v>120</v>
+        <v>423</v>
       </c>
       <c r="M4" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="N4" t="s">
         <v>94</v>
       </c>
       <c r="O4" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="P4" t="s">
         <v>95</v>
@@ -4211,7 +4254,7 @@
         <v>98</v>
       </c>
       <c r="V4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="W4">
         <v>234</v>
@@ -4229,7 +4272,7 @@
         <v>117</v>
       </c>
       <c r="AB4" t="s">
-        <v>233</v>
+        <v>424</v>
       </c>
       <c r="AC4">
         <v>45</v>
@@ -4238,7 +4281,7 @@
         <v>119</v>
       </c>
       <c r="AE4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="AF4" t="s">
         <v>235</v>
@@ -4255,53 +4298,53 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D5" t="s">
         <v>307</v>
       </c>
-      <c r="B5" t="s">
-        <v>306</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D5" t="s">
-        <v>308</v>
-      </c>
       <c r="AJ5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D6" t="s">
         <v>310</v>
       </c>
-      <c r="B6" t="s">
-        <v>306</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D6" t="s">
-        <v>311</v>
-      </c>
       <c r="AJ6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F7" t="s">
         <v>322</v>
-      </c>
-      <c r="F7" t="s">
-        <v>323</v>
       </c>
       <c r="G7" t="s">
         <v>89</v>
@@ -4310,7 +4353,7 @@
         <v>90</v>
       </c>
       <c r="I7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J7" t="s">
         <v>63</v>
@@ -4319,22 +4362,22 @@
         <v>93</v>
       </c>
       <c r="L7" t="s">
-        <v>120</v>
+        <v>423</v>
       </c>
       <c r="M7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N7" t="s">
         <v>94</v>
       </c>
       <c r="O7" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="P7" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="R7" t="s">
         <v>97</v>
@@ -4349,7 +4392,7 @@
         <v>98</v>
       </c>
       <c r="V7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="W7">
         <v>234</v>
@@ -4367,7 +4410,7 @@
         <v>117</v>
       </c>
       <c r="AB7" t="s">
-        <v>233</v>
+        <v>424</v>
       </c>
       <c r="AC7">
         <v>101</v>
@@ -4376,7 +4419,7 @@
         <v>119</v>
       </c>
       <c r="AE7" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AF7" t="s">
         <v>235</v>
@@ -4393,36 +4436,36 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AJ8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AJ9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AK9">
         <v>23.33</v>
@@ -4434,71 +4477,71 @@
         <v>2018</v>
       </c>
       <c r="AN9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D10" t="s">
-        <v>337</v>
-      </c>
-      <c r="F10" t="s">
-        <v>338</v>
+        <v>336</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>426</v>
       </c>
       <c r="AO10" t="s">
+        <v>352</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>347</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>348</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>427</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>349</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>353</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>428</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>429</v>
+      </c>
+      <c r="AX10" t="s">
         <v>354</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>348</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>349</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>353</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>350</v>
-      </c>
-      <c r="AT10" t="s">
-        <v>355</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>351</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>356</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>357</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B11" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D11" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F11" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G11" t="s">
         <v>89</v>
@@ -4516,16 +4559,16 @@
         <v>93</v>
       </c>
       <c r="L11" t="s">
-        <v>120</v>
+        <v>423</v>
       </c>
       <c r="M11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N11" t="s">
         <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="P11" t="s">
         <v>95</v>
@@ -4564,7 +4607,7 @@
         <v>117</v>
       </c>
       <c r="AB11" t="s">
-        <v>233</v>
+        <v>424</v>
       </c>
       <c r="AC11">
         <v>45</v>
@@ -4573,7 +4616,7 @@
         <v>119</v>
       </c>
       <c r="AE11" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AF11" t="s">
         <v>235</v>
@@ -4590,71 +4633,79 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D12" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E12" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F12" t="s">
-        <v>373</v>
+        <v>369</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B13" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D13" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E13" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B14" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D14" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F14" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="AJ14" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="AK14">
         <v>345</v>
       </c>
       <c r="AL14" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="AM14">
         <v>2020</v>
       </c>
       <c r="AN14" t="s">
-        <v>385</v>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -4675,16 +4726,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4702,7 +4755,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F1" t="s">
         <v>54</v>
@@ -4732,7 +4785,7 @@
         <v>62</v>
       </c>
       <c r="O1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -4743,7 +4796,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -4752,7 +4805,7 @@
         <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>421</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4778,22 +4831,22 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F3" t="s">
         <v>297</v>
       </c>
-      <c r="F3" t="s">
-        <v>298</v>
-      </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>421</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -4811,7 +4864,7 @@
         <v>253</v>
       </c>
       <c r="M3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N3" t="s">
         <v>66</v>
@@ -4819,23 +4872,27 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" t="s">
         <v>300</v>
       </c>
-      <c r="B4" t="s">
-        <v>301</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D4" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+      <c r="F4" t="s">
+        <v>422</v>
       </c>
       <c r="O4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4912,10 +4969,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E2" t="s">
         <v>237</v>
@@ -4962,9 +5019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AG12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5013,7 +5068,7 @@
         <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G1" t="s">
         <v>127</v>
@@ -5082,19 +5137,19 @@
         <v>187</v>
       </c>
       <c r="AC1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AD1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AE1" t="s">
         <v>261</v>
       </c>
-      <c r="AE1" t="s">
-        <v>262</v>
-      </c>
       <c r="AF1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AG1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -5105,7 +5160,7 @@
         <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>146</v>
@@ -5176,13 +5231,13 @@
         <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
         <v>183</v>
       </c>
       <c r="E3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H3" t="s">
         <v>167</v>
@@ -5205,7 +5260,7 @@
         <v>180</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D4" t="s">
         <v>184</v>
@@ -5231,7 +5286,7 @@
         <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D5" t="s">
         <v>184</v>
@@ -5240,7 +5295,7 @@
         <v>185</v>
       </c>
       <c r="F5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G5" t="s">
         <v>63</v>
@@ -5254,22 +5309,22 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D6" t="s">
         <v>257</v>
       </c>
-      <c r="B6" t="s">
-        <v>257</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D6" t="s">
-        <v>258</v>
-      </c>
       <c r="E6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K6" t="s">
         <v>154</v>
@@ -5278,33 +5333,33 @@
         <v>158</v>
       </c>
       <c r="AC6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AD6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AE6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AF6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E7" t="s">
         <v>274</v>
-      </c>
-      <c r="E7" t="s">
-        <v>275</v>
       </c>
       <c r="K7" t="s">
         <v>154</v>
@@ -5313,79 +5368,79 @@
         <v>188</v>
       </c>
       <c r="AB7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D8" t="s">
         <v>273</v>
       </c>
-      <c r="B8" t="s">
-        <v>272</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>274</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>275</v>
       </c>
-      <c r="F8" t="s">
-        <v>276</v>
-      </c>
       <c r="K8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AA8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D9" t="s">
         <v>280</v>
       </c>
-      <c r="B9" t="s">
-        <v>280</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>281</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>282</v>
       </c>
-      <c r="F9" t="s">
+      <c r="K9" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA9" t="s">
         <v>283</v>
       </c>
-      <c r="K9" t="s">
-        <v>279</v>
-      </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>284</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D10" t="s">
         <v>182</v>
       </c>
       <c r="E10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K10" t="s">
         <v>154</v>
@@ -5399,39 +5454,39 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B12" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D12" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
       </c>
       <c r="AG12" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -5477,7 +5532,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -5491,7 +5546,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
         <v>102</v>
@@ -5551,7 +5606,7 @@
         <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -5568,7 +5623,7 @@
         <v>224</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D3" t="s">
         <v>223</v>
@@ -5585,7 +5640,7 @@
         <v>226</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D4" t="s">
         <v>227</v>
@@ -5602,7 +5657,7 @@
         <v>229</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D5" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
framework not supporting phone no, made code changes to support
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vamsi Vempati\git\SantoshLatestZahid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vempv\git\LatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF16843-848F-473D-B7F1-09DABAC2C669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D46DAB-14B4-45E8-9834-388FA51C77A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="429">
   <si>
     <t>Environment</t>
   </si>
@@ -1315,9 +1315,6 @@
   </si>
   <si>
     <t>Hussin, Zahid (usaidtest3@gmail.com)</t>
-  </si>
-  <si>
-    <t>YES</t>
   </si>
   <si>
     <t>Activity glaas 10/5</t>
@@ -1764,24 +1761,24 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="66" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +1819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1874,16 +1871,16 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1909,7 +1906,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1935,7 +1932,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C3" s="1"/>
     </row>
   </sheetData>
@@ -1951,19 +1948,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.81640625" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1989,7 +1986,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2007,7 +2004,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>287</v>
       </c>
@@ -2027,7 +2024,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -2060,17 +2057,17 @@
       <selection activeCell="C6" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2111,7 +2108,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -2137,7 +2134,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -2157,7 +2154,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -2180,7 +2177,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -2203,7 +2200,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>355</v>
       </c>
@@ -2246,14 +2243,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2285,7 +2282,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -2326,25 +2323,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -2376,7 +2373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2405,7 +2402,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2434,7 +2431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2463,7 +2460,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2492,7 +2489,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2521,7 +2518,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2550,7 +2547,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2579,7 +2576,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2608,7 +2605,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2637,7 +2634,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2654,7 +2651,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -2666,7 +2663,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2683,7 +2680,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -2695,7 +2692,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2724,7 +2721,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2753,7 +2750,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2782,7 +2779,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2840,7 +2837,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2869,7 +2866,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2898,7 +2895,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2927,7 +2924,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2956,7 +2953,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2985,7 +2982,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3014,7 +3011,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3043,7 +3040,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3072,7 +3069,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3101,7 +3098,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3130,7 +3127,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3159,7 +3156,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3188,7 +3185,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3217,7 +3214,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3246,7 +3243,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3275,7 +3272,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3304,7 +3301,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3333,7 +3330,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3362,7 +3359,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3391,7 +3388,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3420,7 +3417,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3449,7 +3446,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3478,7 +3475,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3507,7 +3504,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3536,7 +3533,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3562,7 +3559,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3591,7 +3588,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3620,7 +3617,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3663,24 +3660,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3724,7 +3721,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>386</v>
       </c>
@@ -3756,7 +3753,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>396</v>
       </c>
@@ -3773,7 +3770,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>402</v>
       </c>
@@ -3818,63 +3815,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="AW10" sqref="AW10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.7265625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="61.26953125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4026,7 +4023,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -4079,16 +4076,16 @@
         <v>97</v>
       </c>
       <c r="S2">
-        <v>98765438</v>
+        <v>987654</v>
       </c>
       <c r="T2">
-        <v>2113</v>
+        <v>211</v>
       </c>
       <c r="U2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4141,7 +4138,7 @@
         <v>97</v>
       </c>
       <c r="S3">
-        <v>98765438</v>
+        <v>987654</v>
       </c>
       <c r="T3">
         <v>211</v>
@@ -4192,7 +4189,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>305</v>
       </c>
@@ -4245,7 +4242,7 @@
         <v>97</v>
       </c>
       <c r="S4">
-        <v>98765438</v>
+        <v>987654</v>
       </c>
       <c r="T4">
         <v>211</v>
@@ -4296,7 +4293,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>306</v>
       </c>
@@ -4313,7 +4310,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>309</v>
       </c>
@@ -4330,7 +4327,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>316</v>
       </c>
@@ -4434,7 +4431,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>317</v>
       </c>
@@ -4451,7 +4448,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>318</v>
       </c>
@@ -4480,7 +4477,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>334</v>
       </c>
@@ -4494,7 +4491,7 @@
         <v>336</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AO10" t="s">
         <v>352</v>
@@ -4506,7 +4503,7 @@
         <v>348</v>
       </c>
       <c r="AR10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AS10" t="s">
         <v>349</v>
@@ -4518,16 +4515,16 @@
         <v>350</v>
       </c>
       <c r="AV10" t="s">
+        <v>427</v>
+      </c>
+      <c r="AW10" t="s">
         <v>428</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>429</v>
       </c>
       <c r="AX10" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>366</v>
       </c>
@@ -4631,7 +4628,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>367</v>
       </c>
@@ -4654,7 +4651,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>370</v>
       </c>
@@ -4671,7 +4668,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>377</v>
       </c>
@@ -4703,7 +4700,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F19" t="s">
         <v>337</v>
       </c>
@@ -4730,18 +4727,18 @@
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4788,7 +4785,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -4829,7 +4826,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>300</v>
       </c>
@@ -4870,7 +4867,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -4904,23 +4901,23 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4961,7 +4958,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -5002,7 +4999,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
@@ -5021,37 +5018,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -5152,7 +5149,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -5223,7 +5220,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -5252,7 +5249,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -5278,7 +5275,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -5307,7 +5304,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>256</v>
       </c>
@@ -5345,7 +5342,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>271</v>
       </c>
@@ -5371,7 +5368,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -5397,7 +5394,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>279</v>
       </c>
@@ -5426,7 +5423,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>331</v>
       </c>
@@ -5452,7 +5449,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>330</v>
       </c>
@@ -5469,7 +5466,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>410</v>
       </c>
@@ -5503,14 +5500,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1796875" customWidth="1"/>
+    <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -5524,7 +5521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -5538,7 +5535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -5552,7 +5549,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C4" s="1"/>
     </row>
   </sheetData>
@@ -5569,16 +5566,16 @@
       <selection activeCell="C5" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -5598,7 +5595,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -5615,7 +5612,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>224</v>
       </c>
@@ -5632,7 +5629,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -5649,7 +5646,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Changed the main neccessary code changes
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vempv\git\LatestDis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D46DAB-14B4-45E8-9834-388FA51C77A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Activity!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1332,8 +1326,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1477,7 +1471,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1509,27 +1503,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1561,24 +1537,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1754,31 +1712,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="66" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1819,7 +1777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1864,23 +1822,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="108" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1906,7 +1864,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1932,7 +1890,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="C3" s="1"/>
     </row>
   </sheetData>
@@ -1941,26 +1899,26 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1986,7 +1944,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2004,7 +1962,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>287</v>
       </c>
@@ -2024,7 +1982,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -2050,24 +2008,24 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2108,7 +2066,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -2134,7 +2092,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -2154,7 +2112,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -2177,7 +2135,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -2200,7 +2158,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>355</v>
       </c>
@@ -2236,21 +2194,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2282,7 +2240,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -2320,28 +2278,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -2373,7 +2331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2390,7 +2348,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -2402,7 +2360,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2419,7 +2377,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
@@ -2431,7 +2389,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2448,7 +2406,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -2460,7 +2418,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2477,7 +2435,7 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -2489,7 +2447,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2506,7 +2464,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
@@ -2518,7 +2476,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2535,7 +2493,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -2547,7 +2505,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2576,7 +2534,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2593,7 +2551,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -2605,7 +2563,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2622,7 +2580,7 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
@@ -2634,7 +2592,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2663,7 +2621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2680,7 +2638,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -2692,7 +2650,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2721,7 +2679,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2750,7 +2708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2779,7 +2737,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2808,7 +2766,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2837,7 +2795,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2866,7 +2824,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2895,7 +2853,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2924,7 +2882,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2953,7 +2911,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2982,7 +2940,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3011,7 +2969,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3040,7 +2998,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3069,7 +3027,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3098,7 +3056,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3127,7 +3085,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3156,7 +3114,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3185,7 +3143,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3214,7 +3172,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3243,7 +3201,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3272,7 +3230,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3301,7 +3259,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3330,7 +3288,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3359,7 +3317,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3388,7 +3346,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3417,7 +3375,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3446,7 +3404,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3475,7 +3433,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3504,7 +3462,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3533,7 +3491,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3559,7 +3517,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3588,7 +3546,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3617,7 +3575,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3653,31 +3611,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3721,7 +3679,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>386</v>
       </c>
@@ -3753,7 +3711,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>396</v>
       </c>
@@ -3770,7 +3728,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>402</v>
       </c>
@@ -3804,7 +3762,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="I4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3812,66 +3770,66 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AX19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.54296875" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="61.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4023,7 +3981,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -4085,7 +4043,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4189,7 +4147,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50">
       <c r="A4" t="s">
         <v>305</v>
       </c>
@@ -4293,7 +4251,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50">
       <c r="A5" t="s">
         <v>306</v>
       </c>
@@ -4310,7 +4268,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50">
       <c r="A6" t="s">
         <v>309</v>
       </c>
@@ -4327,7 +4285,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:50">
       <c r="A7" t="s">
         <v>316</v>
       </c>
@@ -4431,7 +4389,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:50">
       <c r="A8" t="s">
         <v>317</v>
       </c>
@@ -4448,7 +4406,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50">
       <c r="A9" t="s">
         <v>318</v>
       </c>
@@ -4477,7 +4435,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" ht="15.75">
       <c r="A10" t="s">
         <v>334</v>
       </c>
@@ -4524,7 +4482,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50">
       <c r="A11" t="s">
         <v>366</v>
       </c>
@@ -4628,7 +4586,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:50">
       <c r="A12" t="s">
         <v>367</v>
       </c>
@@ -4651,7 +4609,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:50">
       <c r="A13" t="s">
         <v>370</v>
       </c>
@@ -4668,7 +4626,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:50">
       <c r="A14" t="s">
         <v>377</v>
       </c>
@@ -4700,19 +4658,19 @@
         <v>381</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:6">
       <c r="F19" t="s">
         <v>337</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U2" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:U2"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="Q3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="Q4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="Q7" r:id="rId4" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="Q11" r:id="rId5" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="Q3" r:id="rId2"/>
+    <hyperlink ref="Q4" r:id="rId3"/>
+    <hyperlink ref="Q7" r:id="rId4"/>
+    <hyperlink ref="Q11" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -4720,25 +4678,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="32.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4785,7 +4743,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -4826,7 +4784,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>300</v>
       </c>
@@ -4867,7 +4825,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -4894,30 +4852,30 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.54296875" customWidth="1"/>
-    <col min="5" max="5" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4958,7 +4916,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -4999,56 +4957,56 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{1208683C-2B6E-4800-806B-E9EBF668799B}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -5149,7 +5107,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -5220,7 +5178,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -5249,7 +5207,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -5275,7 +5233,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -5304,7 +5262,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>256</v>
       </c>
@@ -5342,7 +5300,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>271</v>
       </c>
@@ -5368,7 +5326,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -5394,7 +5352,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
         <v>279</v>
       </c>
@@ -5423,7 +5381,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>331</v>
       </c>
@@ -5449,7 +5407,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>330</v>
       </c>
@@ -5466,7 +5424,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
         <v>410</v>
       </c>
@@ -5493,21 +5451,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" customWidth="1"/>
-    <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -5521,7 +5479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -5535,7 +5493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -5549,7 +5507,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="C4" s="1"/>
     </row>
   </sheetData>
@@ -5559,23 +5517,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -5595,7 +5553,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -5612,7 +5570,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>224</v>
       </c>
@@ -5629,7 +5587,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -5646,7 +5604,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
made the code changes for createproject and create project and delink01. and excel cyclic errors.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E641F7-6FC5-45F3-B202-8DC0F40DBEE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392B0682-0571-48A0-A86B-4FBAF4A13029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8790" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="428">
   <si>
     <t>Environment</t>
   </si>
@@ -1326,6 +1326,12 @@
   </si>
   <si>
     <t>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</t>
+  </si>
+  <si>
+    <t>Dhaka110045</t>
+  </si>
+  <si>
+    <t>Dhaka110002</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1866,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,7 +1911,7 @@
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>425</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1946,7 +1952,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,7 +2000,7 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>425</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2012,7 +2018,7 @@
       <c r="B3" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>425</v>
       </c>
       <c r="D3" t="s">
@@ -2032,7 +2038,7 @@
       <c r="B4" t="s">
         <v>290</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>425</v>
       </c>
       <c r="D4" t="s">
@@ -2116,7 +2122,7 @@
       <c r="B2" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>425</v>
       </c>
       <c r="D2" t="s">
@@ -2142,7 +2148,7 @@
       <c r="B3" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>425</v>
       </c>
       <c r="D3" t="s">
@@ -2162,7 +2168,7 @@
       <c r="B4" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>425</v>
       </c>
       <c r="D4" t="s">
@@ -2185,7 +2191,7 @@
       <c r="B5" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>425</v>
       </c>
       <c r="D5" t="s">
@@ -2208,7 +2214,7 @@
       <c r="B6" t="s">
         <v>359</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>425</v>
       </c>
       <c r="D6" t="s">
@@ -2290,7 +2296,7 @@
       <c r="B2" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>425</v>
       </c>
       <c r="D2" t="s">
@@ -2325,7 +2331,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F45"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,7 +2513,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>424</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
@@ -2536,7 +2542,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>424</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -2565,7 +2571,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>424</v>
+        <v>101</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -3658,7 +3664,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3729,9 +3735,8 @@
       <c r="B2" t="s">
         <v>390</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C2" t="s">
+        <v>425</v>
       </c>
       <c r="D2" t="s">
         <v>392</v>
@@ -3762,9 +3767,8 @@
       <c r="B3" t="s">
         <v>400</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C3" t="s">
+        <v>425</v>
       </c>
       <c r="D3" t="s">
         <v>401</v>
@@ -3780,9 +3784,8 @@
       <c r="B4" t="s">
         <v>406</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C4" t="s">
+        <v>425</v>
       </c>
       <c r="D4" t="s">
         <v>408</v>
@@ -3849,13 +3852,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
@@ -4045,9 +4049,8 @@
       <c r="B2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C14" ca="1" si="0">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C2" t="s">
+        <v>425</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -4108,9 +4111,8 @@
       <c r="B3" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C3" t="s">
+        <v>425</v>
       </c>
       <c r="D3" t="s">
         <v>109</v>
@@ -4213,9 +4215,8 @@
       <c r="B4" t="s">
         <v>306</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C4" t="s">
+        <v>425</v>
       </c>
       <c r="D4" t="s">
         <v>308</v>
@@ -4318,9 +4319,8 @@
       <c r="B5" t="s">
         <v>306</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C5" t="s">
+        <v>425</v>
       </c>
       <c r="D5" t="s">
         <v>308</v>
@@ -4336,9 +4336,8 @@
       <c r="B6" t="s">
         <v>306</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C6" t="s">
+        <v>425</v>
       </c>
       <c r="D6" t="s">
         <v>311</v>
@@ -4354,9 +4353,8 @@
       <c r="B7" t="s">
         <v>317</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C7" t="s">
+        <v>425</v>
       </c>
       <c r="D7" t="s">
         <v>322</v>
@@ -4459,9 +4457,8 @@
       <c r="B8" t="s">
         <v>317</v>
       </c>
-      <c r="C8" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C8" t="s">
+        <v>425</v>
       </c>
       <c r="D8" t="s">
         <v>322</v>
@@ -4477,9 +4474,8 @@
       <c r="B9" t="s">
         <v>317</v>
       </c>
-      <c r="C9" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C9" t="s">
+        <v>425</v>
       </c>
       <c r="D9" t="s">
         <v>322</v>
@@ -4507,9 +4503,8 @@
       <c r="B10" t="s">
         <v>335</v>
       </c>
-      <c r="C10" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C10" t="s">
+        <v>425</v>
       </c>
       <c r="D10" t="s">
         <v>337</v>
@@ -4555,9 +4550,8 @@
       <c r="B11" t="s">
         <v>370</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C11" t="s">
+        <v>425</v>
       </c>
       <c r="D11" t="s">
         <v>372</v>
@@ -4660,9 +4654,8 @@
       <c r="B12" t="s">
         <v>370</v>
       </c>
-      <c r="C12" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C12" t="s">
+        <v>425</v>
       </c>
       <c r="D12" t="s">
         <v>372</v>
@@ -4681,9 +4674,8 @@
       <c r="B13" t="s">
         <v>370</v>
       </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C13" t="s">
+        <v>425</v>
       </c>
       <c r="D13" t="s">
         <v>375</v>
@@ -4699,9 +4691,8 @@
       <c r="B14" t="s">
         <v>381</v>
       </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C14" t="s">
+        <v>425</v>
       </c>
       <c r="D14" t="s">
         <v>380</v>
@@ -4733,10 +4724,9 @@
     <hyperlink ref="Q4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
     <hyperlink ref="Q7" r:id="rId4" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
     <hyperlink ref="Q11" r:id="rId5" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
-    <hyperlink ref="C2:C14" r:id="rId6" display="usaidtest3@gmail.com/door1room3@#!~Azraq1984@#!" xr:uid="{92100591-A46B-42E3-AB22-DD7BB32AA0A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -4744,16 +4734,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4811,9 +4803,8 @@
       <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C2" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -4822,7 +4813,7 @@
         <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>426</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4853,9 +4844,8 @@
       <c r="B3" t="s">
         <v>301</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C3" t="s">
+        <v>425</v>
       </c>
       <c r="D3" t="s">
         <v>297</v>
@@ -4864,7 +4854,7 @@
         <v>298</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>427</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -4895,9 +4885,8 @@
       <c r="B4" t="s">
         <v>301</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C4" t="s">
+        <v>425</v>
       </c>
       <c r="D4" t="s">
         <v>297</v>
@@ -4907,7 +4896,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{90F5604B-4656-4EE6-BDAA-21C7FFFDEFF1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5035,13 +5028,13 @@
   <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -5176,9 +5169,8 @@
       <c r="B2" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C12" ca="1" si="0">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C2" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D2" t="s">
         <v>146</v>
@@ -5248,9 +5240,8 @@
       <c r="B3" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C3" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D3" t="s">
         <v>183</v>
@@ -5278,9 +5269,8 @@
       <c r="B4" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C4" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D4" t="s">
         <v>184</v>
@@ -5305,9 +5295,8 @@
       <c r="B5" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C5" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D5" t="s">
         <v>184</v>
@@ -5335,9 +5324,8 @@
       <c r="B6" t="s">
         <v>257</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C6" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D6" t="s">
         <v>258</v>
@@ -5374,9 +5362,8 @@
       <c r="B7" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C7" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D7" t="s">
         <v>274</v>
@@ -5401,9 +5388,8 @@
       <c r="B8" t="s">
         <v>272</v>
       </c>
-      <c r="C8" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C8" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D8" t="s">
         <v>274</v>
@@ -5428,9 +5414,8 @@
       <c r="B9" t="s">
         <v>280</v>
       </c>
-      <c r="C9" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C9" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D9" t="s">
         <v>281</v>
@@ -5458,9 +5443,8 @@
       <c r="B10" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C10" t="s">
+        <v>425</v>
       </c>
       <c r="D10" t="s">
         <v>182</v>
@@ -5485,9 +5469,8 @@
       <c r="B11" t="s">
         <v>331</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C11" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D11" t="s">
         <v>329</v>
@@ -5503,9 +5486,8 @@
       <c r="B12" t="s">
         <v>414</v>
       </c>
-      <c r="C12" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C12" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="D12" t="s">
         <v>416</v>
@@ -5524,8 +5506,20 @@
       <c r="C14" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{98C4D12B-7A69-46A9-8355-498EEF14AC8C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{9D9D7178-E857-4022-BA05-BB80DC176F08}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{F0A2B934-AD6C-4159-8B76-9FDC009DA99A}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{022C9D02-DC72-4171-9587-2F8D39E17DAC}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{EEAE20E0-197E-42C5-9CE4-5B0897D16859}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{96A50055-1812-4A49-806D-685C2003DB3F}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{9C104820-14C8-4422-988D-CD5FB675A048}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{53401E5C-01CE-432D-B137-872FB1DCE7D1}"/>
+    <hyperlink ref="C11" r:id="rId9" xr:uid="{36C480B7-B1C7-42FE-AA40-10764A9CABDA}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{F73A1802-C4B7-4450-A899-E1092F4EB796}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -5534,7 +5528,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5565,9 +5559,8 @@
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C2" t="s">
+        <v>425</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -5580,9 +5573,8 @@
       <c r="B3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C3" t="s">
+        <v>425</v>
       </c>
       <c r="D3" t="s">
         <v>102</v>
@@ -5602,7 +5594,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5641,7 +5633,7 @@
       <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="1" t="str">
+      <c r="C2" t="str">
         <f ca="1">$C$3</f>
         <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
       </c>
@@ -5659,7 +5651,7 @@
       <c r="B3" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="1" t="str">
+      <c r="C3" t="str">
         <f ca="1">$C$3</f>
         <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
       </c>
@@ -5677,7 +5669,7 @@
       <c r="B4" t="s">
         <v>226</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C4" t="str">
         <f ca="1">$C$3</f>
         <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
       </c>
@@ -5695,7 +5687,7 @@
       <c r="B5" t="s">
         <v>229</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C5" t="str">
         <f ca="1">$C$3</f>
         <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
       </c>

</xml_diff>

<commit_message>
made code changes to refresh the landingpage.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5A1598-75CE-4197-B34B-6A3DB71F53E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A890C7-4FBB-49D6-89D9-6F5CE5C4C62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="8760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="432">
   <si>
     <t>Environment</t>
   </si>
@@ -1058,9 +1058,6 @@
     <t>Add funding strip details</t>
   </si>
   <si>
-    <t>James15930</t>
-  </si>
-  <si>
     <t>SourceOfFunding</t>
   </si>
   <si>
@@ -1341,6 +1338,12 @@
   </si>
   <si>
     <t>MccM1359</t>
+  </si>
+  <si>
+    <t>Brackin, James (jbrackin@usaid.gov)</t>
+  </si>
+  <si>
+    <t>Activity glaas 10/5</t>
   </si>
 </sst>
 </file>
@@ -1838,7 +1841,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1847,7 +1850,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G2">
         <v>45</v>
@@ -1862,7 +1865,7 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1928,7 +1931,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
@@ -2017,7 +2020,7 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>47</v>
@@ -2035,7 +2038,7 @@
         <v>286</v>
       </c>
       <c r="C3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>289</v>
@@ -2055,7 +2058,7 @@
         <v>288</v>
       </c>
       <c r="C4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
         <v>290</v>
@@ -2122,13 +2125,13 @@
         <v>217</v>
       </c>
       <c r="K1" t="s">
+        <v>360</v>
+      </c>
+      <c r="L1" t="s">
         <v>361</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>362</v>
-      </c>
-      <c r="M1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -2139,7 +2142,7 @@
         <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
         <v>172</v>
@@ -2165,7 +2168,7 @@
         <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>195</v>
@@ -2185,7 +2188,7 @@
         <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
         <v>197</v>
@@ -2208,7 +2211,7 @@
         <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D5" t="s">
         <v>215</v>
@@ -2225,31 +2228,31 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
+        <v>358</v>
+      </c>
+      <c r="E6" t="s">
         <v>359</v>
       </c>
-      <c r="E6" t="s">
-        <v>360</v>
-      </c>
       <c r="J6" t="s">
+        <v>363</v>
+      </c>
+      <c r="K6" t="s">
         <v>364</v>
       </c>
-      <c r="K6" t="s">
-        <v>365</v>
-      </c>
       <c r="L6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -2313,7 +2316,7 @@
         <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
         <v>211</v>
@@ -2347,7 +2350,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2558,7 +2561,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -2616,7 +2619,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -2674,7 +2677,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>422</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -2703,7 +2706,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -2732,7 +2735,7 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
@@ -2761,7 +2764,7 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -2790,7 +2793,7 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -2819,7 +2822,7 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
@@ -2848,7 +2851,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -2877,7 +2880,7 @@
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
@@ -2894,7 +2897,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C19" t="s">
         <v>114</v>
@@ -2906,7 +2909,7 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>
@@ -2923,19 +2926,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C20" t="s">
+        <v>365</v>
+      </c>
+      <c r="D20" t="s">
         <v>366</v>
-      </c>
-      <c r="D20" t="s">
-        <v>367</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
@@ -2952,19 +2955,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>371</v>
+      </c>
+      <c r="C21" t="s">
+        <v>365</v>
+      </c>
+      <c r="D21" t="s">
         <v>372</v>
-      </c>
-      <c r="C21" t="s">
-        <v>366</v>
-      </c>
-      <c r="D21" t="s">
-        <v>373</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G21" t="s">
         <v>24</v>
@@ -2981,19 +2984,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C22" t="s">
         <v>318</v>
       </c>
       <c r="D22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
@@ -3022,7 +3025,7 @@
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
@@ -3051,7 +3054,7 @@
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
@@ -3080,7 +3083,7 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G25" t="s">
         <v>24</v>
@@ -3109,7 +3112,7 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G26" t="s">
         <v>24</v>
@@ -3138,7 +3141,7 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
@@ -3167,7 +3170,7 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G28" t="s">
         <v>24</v>
@@ -3196,7 +3199,7 @@
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
@@ -3225,7 +3228,7 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
@@ -3254,7 +3257,7 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G31" t="s">
         <v>24</v>
@@ -3283,7 +3286,7 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -3300,19 +3303,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>411</v>
+      </c>
+      <c r="C33" t="s">
         <v>412</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>413</v>
-      </c>
-      <c r="D33" t="s">
-        <v>414</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G33" t="s">
         <v>24</v>
@@ -3341,7 +3344,7 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G34" t="s">
         <v>24</v>
@@ -3370,7 +3373,7 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
@@ -3399,7 +3402,7 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G36" t="s">
         <v>24</v>
@@ -3416,19 +3419,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>356</v>
+      </c>
+      <c r="C37" t="s">
         <v>357</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>358</v>
-      </c>
-      <c r="D37" t="s">
-        <v>359</v>
       </c>
       <c r="E37" t="s">
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G37" t="s">
         <v>24</v>
@@ -3457,7 +3460,7 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G38" t="s">
         <v>24</v>
@@ -3486,7 +3489,7 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
@@ -3515,7 +3518,7 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G40" t="s">
         <v>24</v>
@@ -3544,7 +3547,7 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G41" t="s">
         <v>24</v>
@@ -3573,7 +3576,7 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H42" t="s">
         <v>238</v>
@@ -3587,28 +3590,28 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>387</v>
+      </c>
+      <c r="C43" t="s">
         <v>388</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>389</v>
-      </c>
-      <c r="D43" t="s">
-        <v>390</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G43" t="s">
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -3616,28 +3619,28 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>397</v>
+      </c>
+      <c r="C44" t="s">
+        <v>399</v>
+      </c>
+      <c r="D44" t="s">
         <v>398</v>
-      </c>
-      <c r="C44" t="s">
-        <v>400</v>
-      </c>
-      <c r="D44" t="s">
-        <v>399</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G44" t="s">
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I44" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3645,28 +3648,28 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>403</v>
+      </c>
+      <c r="C45" t="s">
         <v>404</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>405</v>
-      </c>
-      <c r="D45" t="s">
-        <v>406</v>
       </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G45" t="s">
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I45" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -3717,109 +3720,109 @@
         <v>268</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>196</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="J1" t="s">
         <v>386</v>
       </c>
-      <c r="J1" t="s">
-        <v>387</v>
-      </c>
       <c r="K1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M1" t="s">
+        <v>400</v>
+      </c>
+      <c r="N1" t="s">
         <v>402</v>
-      </c>
-      <c r="M1" t="s">
-        <v>401</v>
-      </c>
-      <c r="N1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
       </c>
       <c r="I2" t="s">
+        <v>392</v>
+      </c>
+      <c r="J2" t="s">
         <v>393</v>
       </c>
-      <c r="J2" t="s">
-        <v>394</v>
-      </c>
       <c r="K2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D3" t="s">
         <v>398</v>
       </c>
-      <c r="B3" t="s">
-        <v>398</v>
-      </c>
-      <c r="C3" t="s">
-        <v>423</v>
-      </c>
-      <c r="D3" t="s">
-        <v>399</v>
-      </c>
       <c r="K3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F4" t="s">
         <v>406</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>407</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" t="s">
+        <v>410</v>
+      </c>
+      <c r="M4" t="s">
         <v>409</v>
-      </c>
-      <c r="L4" t="s">
-        <v>411</v>
-      </c>
-      <c r="M4" t="s">
-        <v>410</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -3868,8 +3871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4028,34 +4031,34 @@
         <v>314</v>
       </c>
       <c r="AO1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AP1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>337</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>338</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>339</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>340</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>341</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>342</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>343</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>344</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.35">
@@ -4066,7 +4069,7 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -4090,16 +4093,16 @@
         <v>93</v>
       </c>
       <c r="L2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M2" t="s">
         <v>426</v>
-      </c>
-      <c r="M2" t="s">
-        <v>427</v>
       </c>
       <c r="N2" t="s">
         <v>94</v>
       </c>
       <c r="O2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P2" t="s">
         <v>95</v>
@@ -4120,7 +4123,7 @@
         <v>98</v>
       </c>
       <c r="AB2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.35">
@@ -4131,7 +4134,7 @@
         <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>109</v>
@@ -4155,16 +4158,16 @@
         <v>93</v>
       </c>
       <c r="L3" t="s">
+        <v>425</v>
+      </c>
+      <c r="M3" t="s">
         <v>426</v>
-      </c>
-      <c r="M3" t="s">
-        <v>427</v>
       </c>
       <c r="N3" t="s">
         <v>94</v>
       </c>
       <c r="O3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P3" t="s">
         <v>95</v>
@@ -4203,7 +4206,7 @@
         <v>117</v>
       </c>
       <c r="AB3" t="s">
-        <v>233</v>
+        <v>430</v>
       </c>
       <c r="AC3">
         <v>45</v>
@@ -4212,7 +4215,7 @@
         <v>119</v>
       </c>
       <c r="AE3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF3" t="s">
         <v>235</v>
@@ -4235,7 +4238,7 @@
         <v>304</v>
       </c>
       <c r="C4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
         <v>306</v>
@@ -4262,13 +4265,13 @@
         <v>120</v>
       </c>
       <c r="M4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N4" t="s">
         <v>94</v>
       </c>
       <c r="O4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P4" t="s">
         <v>95</v>
@@ -4316,7 +4319,7 @@
         <v>119</v>
       </c>
       <c r="AE4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF4" t="s">
         <v>235</v>
@@ -4339,7 +4342,7 @@
         <v>304</v>
       </c>
       <c r="C5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D5" t="s">
         <v>306</v>
@@ -4356,7 +4359,7 @@
         <v>304</v>
       </c>
       <c r="C6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
         <v>309</v>
@@ -4373,7 +4376,7 @@
         <v>315</v>
       </c>
       <c r="C7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D7" t="s">
         <v>320</v>
@@ -4400,13 +4403,13 @@
         <v>120</v>
       </c>
       <c r="M7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N7" t="s">
         <v>94</v>
       </c>
       <c r="O7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P7" t="s">
         <v>323</v>
@@ -4454,7 +4457,7 @@
         <v>119</v>
       </c>
       <c r="AE7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AF7" t="s">
         <v>235</v>
@@ -4477,7 +4480,7 @@
         <v>315</v>
       </c>
       <c r="C8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D8" t="s">
         <v>320</v>
@@ -4494,7 +4497,7 @@
         <v>315</v>
       </c>
       <c r="C9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D9" t="s">
         <v>320</v>
@@ -4523,60 +4526,60 @@
         <v>333</v>
       </c>
       <c r="C10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D10" t="s">
         <v>335</v>
       </c>
       <c r="F10" t="s">
-        <v>336</v>
+        <v>431</v>
       </c>
       <c r="AO10" t="s">
+        <v>351</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>345</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>346</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>350</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>347</v>
+      </c>
+      <c r="AT10" t="s">
         <v>352</v>
       </c>
-      <c r="AP10" t="s">
-        <v>346</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>347</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>351</v>
-      </c>
-      <c r="AS10" t="s">
+      <c r="AU10" t="s">
         <v>348</v>
       </c>
-      <c r="AT10" t="s">
+      <c r="AV10" t="s">
         <v>353</v>
       </c>
-      <c r="AU10" t="s">
-        <v>349</v>
-      </c>
-      <c r="AV10" t="s">
+      <c r="AW10" t="s">
         <v>354</v>
       </c>
-      <c r="AW10" t="s">
+      <c r="AX10" t="s">
         <v>355</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D11" t="s">
+        <v>369</v>
+      </c>
+      <c r="F11" t="s">
         <v>370</v>
-      </c>
-      <c r="F11" t="s">
-        <v>371</v>
       </c>
       <c r="G11" t="s">
         <v>89</v>
@@ -4597,13 +4600,13 @@
         <v>120</v>
       </c>
       <c r="M11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N11" t="s">
         <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P11" t="s">
         <v>95</v>
@@ -4651,7 +4654,7 @@
         <v>119</v>
       </c>
       <c r="AE11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AF11" t="s">
         <v>235</v>
@@ -4668,71 +4671,71 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" t="s">
+        <v>367</v>
+      </c>
+      <c r="C12" t="s">
+        <v>422</v>
+      </c>
+      <c r="D12" t="s">
         <v>369</v>
       </c>
-      <c r="B12" t="s">
-        <v>368</v>
-      </c>
-      <c r="C12" t="s">
-        <v>423</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>374</v>
+      </c>
+      <c r="F12" t="s">
         <v>370</v>
-      </c>
-      <c r="E12" t="s">
-        <v>375</v>
-      </c>
-      <c r="F12" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>371</v>
+      </c>
+      <c r="B13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C13" t="s">
+        <v>422</v>
+      </c>
+      <c r="D13" t="s">
         <v>372</v>
       </c>
-      <c r="B13" t="s">
-        <v>368</v>
-      </c>
-      <c r="C13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>373</v>
-      </c>
-      <c r="E13" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B14" t="s">
+        <v>378</v>
+      </c>
+      <c r="C14" t="s">
+        <v>422</v>
+      </c>
+      <c r="D14" t="s">
+        <v>377</v>
+      </c>
+      <c r="F14" t="s">
         <v>379</v>
       </c>
-      <c r="B14" t="s">
-        <v>379</v>
-      </c>
-      <c r="C14" t="s">
-        <v>423</v>
-      </c>
-      <c r="D14" t="s">
-        <v>378</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="AJ14" t="s">
         <v>380</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>381</v>
       </c>
       <c r="AK14">
         <v>345</v>
       </c>
       <c r="AL14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AM14">
         <v>2020</v>
       </c>
       <c r="AN14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4824,7 +4827,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -4833,7 +4836,7 @@
         <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4865,7 +4868,7 @@
         <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>295</v>
@@ -4874,7 +4877,7 @@
         <v>296</v>
       </c>
       <c r="G3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -4906,13 +4909,13 @@
         <v>299</v>
       </c>
       <c r="C4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
         <v>295</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O4" t="s">
         <v>301</v>
@@ -5000,10 +5003,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="E2" t="s">
         <v>237</v>
@@ -5182,7 +5185,7 @@
         <v>262</v>
       </c>
       <c r="AG1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
@@ -5193,7 +5196,7 @@
         <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
         <v>146</v>
@@ -5264,7 +5267,7 @@
         <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>183</v>
@@ -5293,7 +5296,7 @@
         <v>180</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
         <v>184</v>
@@ -5319,7 +5322,7 @@
         <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D5" t="s">
         <v>184</v>
@@ -5348,7 +5351,7 @@
         <v>255</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
         <v>256</v>
@@ -5386,7 +5389,7 @@
         <v>270</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D7" t="s">
         <v>272</v>
@@ -5412,7 +5415,7 @@
         <v>270</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D8" t="s">
         <v>272</v>
@@ -5438,7 +5441,7 @@
         <v>278</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D9" t="s">
         <v>279</v>
@@ -5467,7 +5470,7 @@
         <v>329</v>
       </c>
       <c r="C10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D10" t="s">
         <v>182</v>
@@ -5493,7 +5496,7 @@
         <v>329</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D11" t="s">
         <v>327</v>
@@ -5504,22 +5507,22 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
       </c>
       <c r="AG12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -5583,7 +5586,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -5597,7 +5600,7 @@
         <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Made code changes for addfundingStrip made sync for other activity tests added delete fundingstrip.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A890C7-4FBB-49D6-89D9-6F5CE5C4C62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF1BDF9-617F-4643-852A-4730F911E0EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="8760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="431">
   <si>
     <t>Environment</t>
   </si>
@@ -1098,9 +1098,6 @@
   </si>
   <si>
     <t>DistribtionCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Democracy &amp; Governance </t>
   </si>
   <si>
     <t>123-M</t>
@@ -1841,7 +1838,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1850,7 +1847,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G2">
         <v>45</v>
@@ -1865,7 +1862,7 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1931,7 +1928,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
@@ -2020,7 +2017,7 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>47</v>
@@ -2038,7 +2035,7 @@
         <v>286</v>
       </c>
       <c r="C3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>289</v>
@@ -2058,7 +2055,7 @@
         <v>288</v>
       </c>
       <c r="C4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
         <v>290</v>
@@ -2125,13 +2122,13 @@
         <v>217</v>
       </c>
       <c r="K1" t="s">
+        <v>359</v>
+      </c>
+      <c r="L1" t="s">
         <v>360</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>361</v>
-      </c>
-      <c r="M1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -2142,7 +2139,7 @@
         <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
         <v>172</v>
@@ -2168,7 +2165,7 @@
         <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>195</v>
@@ -2188,7 +2185,7 @@
         <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
         <v>197</v>
@@ -2211,7 +2208,7 @@
         <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" t="s">
         <v>215</v>
@@ -2228,31 +2225,31 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
+        <v>357</v>
+      </c>
+      <c r="E6" t="s">
         <v>358</v>
       </c>
-      <c r="E6" t="s">
-        <v>359</v>
-      </c>
       <c r="J6" t="s">
+        <v>362</v>
+      </c>
+      <c r="K6" t="s">
         <v>363</v>
       </c>
-      <c r="K6" t="s">
-        <v>364</v>
-      </c>
       <c r="L6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2316,7 +2313,7 @@
         <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
         <v>211</v>
@@ -2350,7 +2347,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2561,7 +2558,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>421</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -2590,7 +2587,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>420</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -2619,7 +2616,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -2706,7 +2703,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>421</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -2735,7 +2732,7 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
@@ -2764,7 +2761,7 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -2793,7 +2790,7 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -2822,7 +2819,7 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
@@ -2851,7 +2848,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -2880,7 +2877,7 @@
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
@@ -2897,7 +2894,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C19" t="s">
         <v>114</v>
@@ -2909,7 +2906,7 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>
@@ -2926,19 +2923,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C20" t="s">
+        <v>364</v>
+      </c>
+      <c r="D20" t="s">
         <v>365</v>
-      </c>
-      <c r="D20" t="s">
-        <v>366</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
@@ -2955,19 +2952,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>370</v>
+      </c>
+      <c r="C21" t="s">
+        <v>364</v>
+      </c>
+      <c r="D21" t="s">
         <v>371</v>
-      </c>
-      <c r="C21" t="s">
-        <v>365</v>
-      </c>
-      <c r="D21" t="s">
-        <v>372</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G21" t="s">
         <v>24</v>
@@ -2984,19 +2981,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C22" t="s">
         <v>318</v>
       </c>
       <c r="D22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
@@ -3025,7 +3022,7 @@
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
@@ -3054,7 +3051,7 @@
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
@@ -3083,7 +3080,7 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G25" t="s">
         <v>24</v>
@@ -3112,7 +3109,7 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G26" t="s">
         <v>24</v>
@@ -3141,7 +3138,7 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
@@ -3170,7 +3167,7 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G28" t="s">
         <v>24</v>
@@ -3199,7 +3196,7 @@
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
@@ -3228,7 +3225,7 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
@@ -3257,7 +3254,7 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G31" t="s">
         <v>24</v>
@@ -3286,7 +3283,7 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -3303,19 +3300,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>410</v>
+      </c>
+      <c r="C33" t="s">
         <v>411</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>412</v>
-      </c>
-      <c r="D33" t="s">
-        <v>413</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G33" t="s">
         <v>24</v>
@@ -3344,7 +3341,7 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G34" t="s">
         <v>24</v>
@@ -3373,7 +3370,7 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
@@ -3402,7 +3399,7 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G36" t="s">
         <v>24</v>
@@ -3419,19 +3416,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>355</v>
+      </c>
+      <c r="C37" t="s">
         <v>356</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>357</v>
-      </c>
-      <c r="D37" t="s">
-        <v>358</v>
       </c>
       <c r="E37" t="s">
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G37" t="s">
         <v>24</v>
@@ -3460,7 +3457,7 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G38" t="s">
         <v>24</v>
@@ -3489,7 +3486,7 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
@@ -3518,7 +3515,7 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G40" t="s">
         <v>24</v>
@@ -3547,7 +3544,7 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G41" t="s">
         <v>24</v>
@@ -3576,7 +3573,7 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H42" t="s">
         <v>238</v>
@@ -3590,28 +3587,28 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>386</v>
+      </c>
+      <c r="C43" t="s">
         <v>387</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>388</v>
-      </c>
-      <c r="D43" t="s">
-        <v>389</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G43" t="s">
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I43" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -3619,28 +3616,28 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>396</v>
+      </c>
+      <c r="C44" t="s">
+        <v>398</v>
+      </c>
+      <c r="D44" t="s">
         <v>397</v>
-      </c>
-      <c r="C44" t="s">
-        <v>399</v>
-      </c>
-      <c r="D44" t="s">
-        <v>398</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G44" t="s">
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I44" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3648,28 +3645,28 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>402</v>
+      </c>
+      <c r="C45" t="s">
         <v>403</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>404</v>
-      </c>
-      <c r="D45" t="s">
-        <v>405</v>
       </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G45" t="s">
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I45" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -3720,109 +3717,109 @@
         <v>268</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>196</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J1" t="s">
         <v>385</v>
       </c>
-      <c r="J1" t="s">
-        <v>386</v>
-      </c>
       <c r="K1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L1" t="s">
+        <v>400</v>
+      </c>
+      <c r="M1" t="s">
+        <v>399</v>
+      </c>
+      <c r="N1" t="s">
         <v>401</v>
-      </c>
-      <c r="M1" t="s">
-        <v>400</v>
-      </c>
-      <c r="N1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
       </c>
       <c r="I2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J2" t="s">
         <v>392</v>
       </c>
-      <c r="J2" t="s">
-        <v>393</v>
-      </c>
       <c r="K2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3" t="s">
         <v>397</v>
       </c>
-      <c r="B3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C3" t="s">
-        <v>422</v>
-      </c>
-      <c r="D3" t="s">
-        <v>398</v>
-      </c>
       <c r="K3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
+        <v>404</v>
+      </c>
+      <c r="F4" t="s">
         <v>405</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>406</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" t="s">
+        <v>409</v>
+      </c>
+      <c r="M4" t="s">
         <v>408</v>
-      </c>
-      <c r="L4" t="s">
-        <v>410</v>
-      </c>
-      <c r="M4" t="s">
-        <v>409</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -3871,9 +3868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AC10" sqref="AC10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4069,7 +4064,7 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -4093,16 +4088,16 @@
         <v>93</v>
       </c>
       <c r="L2" t="s">
+        <v>424</v>
+      </c>
+      <c r="M2" t="s">
         <v>425</v>
-      </c>
-      <c r="M2" t="s">
-        <v>426</v>
       </c>
       <c r="N2" t="s">
         <v>94</v>
       </c>
       <c r="O2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P2" t="s">
         <v>95</v>
@@ -4123,7 +4118,7 @@
         <v>98</v>
       </c>
       <c r="AB2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.35">
@@ -4134,7 +4129,7 @@
         <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>109</v>
@@ -4158,16 +4153,16 @@
         <v>93</v>
       </c>
       <c r="L3" t="s">
+        <v>424</v>
+      </c>
+      <c r="M3" t="s">
         <v>425</v>
-      </c>
-      <c r="M3" t="s">
-        <v>426</v>
       </c>
       <c r="N3" t="s">
         <v>94</v>
       </c>
       <c r="O3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P3" t="s">
         <v>95</v>
@@ -4206,7 +4201,7 @@
         <v>117</v>
       </c>
       <c r="AB3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AC3">
         <v>45</v>
@@ -4215,7 +4210,7 @@
         <v>119</v>
       </c>
       <c r="AE3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF3" t="s">
         <v>235</v>
@@ -4238,7 +4233,7 @@
         <v>304</v>
       </c>
       <c r="C4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
         <v>306</v>
@@ -4265,13 +4260,13 @@
         <v>120</v>
       </c>
       <c r="M4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="N4" t="s">
         <v>94</v>
       </c>
       <c r="O4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P4" t="s">
         <v>95</v>
@@ -4319,7 +4314,7 @@
         <v>119</v>
       </c>
       <c r="AE4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF4" t="s">
         <v>235</v>
@@ -4342,7 +4337,7 @@
         <v>304</v>
       </c>
       <c r="C5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" t="s">
         <v>306</v>
@@ -4359,7 +4354,7 @@
         <v>304</v>
       </c>
       <c r="C6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
         <v>309</v>
@@ -4376,7 +4371,7 @@
         <v>315</v>
       </c>
       <c r="C7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D7" t="s">
         <v>320</v>
@@ -4403,13 +4398,13 @@
         <v>120</v>
       </c>
       <c r="M7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="N7" t="s">
         <v>94</v>
       </c>
       <c r="O7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P7" t="s">
         <v>323</v>
@@ -4457,7 +4452,7 @@
         <v>119</v>
       </c>
       <c r="AE7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF7" t="s">
         <v>235</v>
@@ -4480,7 +4475,7 @@
         <v>315</v>
       </c>
       <c r="C8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D8" t="s">
         <v>320</v>
@@ -4497,7 +4492,7 @@
         <v>315</v>
       </c>
       <c r="C9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D9" t="s">
         <v>320</v>
@@ -4526,16 +4521,16 @@
         <v>333</v>
       </c>
       <c r="C10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D10" t="s">
         <v>335</v>
       </c>
       <c r="F10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AO10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AP10" t="s">
         <v>345</v>
@@ -4544,42 +4539,42 @@
         <v>346</v>
       </c>
       <c r="AR10" t="s">
-        <v>350</v>
+        <v>424</v>
       </c>
       <c r="AS10" t="s">
         <v>347</v>
       </c>
       <c r="AT10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AU10" t="s">
         <v>348</v>
       </c>
       <c r="AV10" t="s">
+        <v>352</v>
+      </c>
+      <c r="AW10" t="s">
         <v>353</v>
       </c>
-      <c r="AW10" t="s">
+      <c r="AX10" t="s">
         <v>354</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D11" t="s">
+        <v>368</v>
+      </c>
+      <c r="F11" t="s">
         <v>369</v>
-      </c>
-      <c r="F11" t="s">
-        <v>370</v>
       </c>
       <c r="G11" t="s">
         <v>89</v>
@@ -4600,13 +4595,13 @@
         <v>120</v>
       </c>
       <c r="M11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="N11" t="s">
         <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P11" t="s">
         <v>95</v>
@@ -4654,7 +4649,7 @@
         <v>119</v>
       </c>
       <c r="AE11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF11" t="s">
         <v>235</v>
@@ -4671,71 +4666,71 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B12" t="s">
+        <v>366</v>
+      </c>
+      <c r="C12" t="s">
+        <v>421</v>
+      </c>
+      <c r="D12" t="s">
         <v>368</v>
       </c>
-      <c r="B12" t="s">
-        <v>367</v>
-      </c>
-      <c r="C12" t="s">
-        <v>422</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>373</v>
+      </c>
+      <c r="F12" t="s">
         <v>369</v>
-      </c>
-      <c r="E12" t="s">
-        <v>374</v>
-      </c>
-      <c r="F12" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" t="s">
+        <v>421</v>
+      </c>
+      <c r="D13" t="s">
         <v>371</v>
       </c>
-      <c r="B13" t="s">
-        <v>367</v>
-      </c>
-      <c r="C13" t="s">
-        <v>422</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>372</v>
-      </c>
-      <c r="E13" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B14" t="s">
+        <v>377</v>
+      </c>
+      <c r="C14" t="s">
+        <v>421</v>
+      </c>
+      <c r="D14" t="s">
+        <v>376</v>
+      </c>
+      <c r="F14" t="s">
         <v>378</v>
       </c>
-      <c r="B14" t="s">
-        <v>378</v>
-      </c>
-      <c r="C14" t="s">
-        <v>422</v>
-      </c>
-      <c r="D14" t="s">
-        <v>377</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="AJ14" t="s">
         <v>379</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>380</v>
       </c>
       <c r="AK14">
         <v>345</v>
       </c>
       <c r="AL14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AM14">
         <v>2020</v>
       </c>
       <c r="AN14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -4827,7 +4822,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -4836,7 +4831,7 @@
         <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4868,7 +4863,7 @@
         <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>295</v>
@@ -4877,7 +4872,7 @@
         <v>296</v>
       </c>
       <c r="G3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -4909,13 +4904,13 @@
         <v>299</v>
       </c>
       <c r="C4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
         <v>295</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="O4" t="s">
         <v>301</v>
@@ -5003,10 +4998,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>417</v>
       </c>
       <c r="E2" t="s">
         <v>237</v>
@@ -5185,7 +5180,7 @@
         <v>262</v>
       </c>
       <c r="AG1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
@@ -5196,7 +5191,7 @@
         <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
         <v>146</v>
@@ -5267,7 +5262,7 @@
         <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>183</v>
@@ -5296,7 +5291,7 @@
         <v>180</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
         <v>184</v>
@@ -5322,7 +5317,7 @@
         <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" t="s">
         <v>184</v>
@@ -5351,7 +5346,7 @@
         <v>255</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
         <v>256</v>
@@ -5389,7 +5384,7 @@
         <v>270</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D7" t="s">
         <v>272</v>
@@ -5415,7 +5410,7 @@
         <v>270</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D8" t="s">
         <v>272</v>
@@ -5441,7 +5436,7 @@
         <v>278</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D9" t="s">
         <v>279</v>
@@ -5470,7 +5465,7 @@
         <v>329</v>
       </c>
       <c r="C10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D10" t="s">
         <v>182</v>
@@ -5496,7 +5491,7 @@
         <v>329</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D11" t="s">
         <v>327</v>
@@ -5507,22 +5502,22 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
       </c>
       <c r="AG12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -5586,7 +5581,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -5600,7 +5595,7 @@
         <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Added  12 and 13 test cases
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF1BDF9-617F-4643-852A-4730F911E0EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3552AA23-000D-443A-A131-602A89CC634A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="8760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21435" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Activity!$A$1:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestSuite!$A$1:$J$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="434">
   <si>
     <t>Environment</t>
   </si>
@@ -1341,6 +1342,15 @@
   </si>
   <si>
     <t>Activity glaas 10/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office name </t>
+  </si>
+  <si>
+    <t>Actiivty name on 10/5</t>
+  </si>
+  <si>
+    <t>PS.3-1</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2357,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2761,7 +2771,7 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -2790,7 +2800,7 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -3216,7 +3226,7 @@
         <v>278</v>
       </c>
       <c r="C30" t="s">
-        <v>181</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
         <v>279</v>
@@ -3868,11 +3878,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AJ6" sqref="AJ6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
@@ -4257,7 +4269,7 @@
         <v>93</v>
       </c>
       <c r="L4" t="s">
-        <v>120</v>
+        <v>431</v>
       </c>
       <c r="M4" t="s">
         <v>425</v>
@@ -4305,7 +4317,7 @@
         <v>117</v>
       </c>
       <c r="AB4" t="s">
-        <v>233</v>
+        <v>429</v>
       </c>
       <c r="AC4">
         <v>45</v>
@@ -4342,8 +4354,11 @@
       <c r="D5" t="s">
         <v>306</v>
       </c>
+      <c r="F5" t="s">
+        <v>432</v>
+      </c>
       <c r="AJ5" t="s">
-        <v>301</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
@@ -4359,8 +4374,11 @@
       <c r="D6" t="s">
         <v>309</v>
       </c>
+      <c r="F6" t="s">
+        <v>432</v>
+      </c>
       <c r="AJ6" t="s">
-        <v>301</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.35">
@@ -5549,7 +5567,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5615,7 +5633,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5654,9 +5672,8 @@
       <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C2" t="s">
+        <v>421</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -5672,9 +5689,8 @@
       <c r="B3" t="s">
         <v>224</v>
       </c>
-      <c r="C3" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C3" t="s">
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>223</v>
@@ -5690,9 +5706,8 @@
       <c r="B4" t="s">
         <v>226</v>
       </c>
-      <c r="C4" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C4" t="s">
+        <v>421</v>
       </c>
       <c r="D4" t="s">
         <v>227</v>
@@ -5708,9 +5723,8 @@
       <c r="B5" t="s">
         <v>229</v>
       </c>
-      <c r="C5" t="str">
-        <f ca="1">$C$3</f>
-        <v>usaidtest3@gmail.com/Azraq1984@#!~door1room3@#!</v>
+      <c r="C5" t="s">
+        <v>421</v>
       </c>
       <c r="D5" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
MADE changes for enivironment
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3552AA23-000D-443A-A131-602A89CC634A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3173F74D-8188-4CE0-9931-67BE399CB39B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21435" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="436">
   <si>
     <t>Environment</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>DIS</t>
-  </si>
-  <si>
     <t>OfficeName</t>
   </si>
   <si>
@@ -1351,6 +1348,15 @@
   </si>
   <si>
     <t>PS.3-1</t>
+  </si>
+  <si>
+    <t>DIS PROD</t>
+  </si>
+  <si>
+    <t>JOHN</t>
+  </si>
+  <si>
+    <t>Agreements (Not BPA BOA or Leases)</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1788,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1845,10 +1851,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>433</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1857,7 +1863,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G2">
         <v>45</v>
@@ -1869,16 +1875,16 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1918,42 +1924,42 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G2" s="3">
         <v>43705</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2007,30 +2013,30 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2039,42 +2045,42 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2114,74 +2120,74 @@
         <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" t="s">
         <v>175</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>176</v>
       </c>
-      <c r="G1" t="s">
-        <v>177</v>
-      </c>
       <c r="H1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" t="s">
         <v>216</v>
       </c>
-      <c r="J1" t="s">
-        <v>217</v>
-      </c>
       <c r="K1" t="s">
+        <v>358</v>
+      </c>
+      <c r="L1" t="s">
         <v>359</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>360</v>
-      </c>
-      <c r="M1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2">
         <v>2017</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F3">
         <v>2019</v>
@@ -2189,77 +2195,77 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4">
         <v>2017</v>
       </c>
       <c r="G4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" t="s">
         <v>214</v>
       </c>
-      <c r="B5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C5" t="s">
-        <v>421</v>
-      </c>
-      <c r="D5" t="s">
-        <v>215</v>
-      </c>
       <c r="E5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I5" t="s">
         <v>218</v>
       </c>
-      <c r="I5" t="s">
-        <v>219</v>
-      </c>
       <c r="J5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D6" t="s">
+        <v>356</v>
+      </c>
+      <c r="E6" t="s">
         <v>357</v>
       </c>
-      <c r="E6" t="s">
-        <v>358</v>
-      </c>
       <c r="J6" t="s">
+        <v>361</v>
+      </c>
+      <c r="K6" t="s">
         <v>362</v>
       </c>
-      <c r="K6" t="s">
-        <v>363</v>
-      </c>
       <c r="L6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -2297,54 +2303,54 @@
         <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" t="s">
         <v>201</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>202</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>203</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>204</v>
-      </c>
-      <c r="J1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D2" t="s">
         <v>210</v>
       </c>
-      <c r="B2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" t="s">
-        <v>421</v>
-      </c>
-      <c r="D2" t="s">
-        <v>211</v>
-      </c>
       <c r="E2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2" t="s">
         <v>206</v>
-      </c>
-      <c r="G2" t="s">
-        <v>207</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J2" t="s">
         <v>208</v>
-      </c>
-      <c r="J2" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2357,7 +2363,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2411,28 +2417,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2440,28 +2446,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -2469,28 +2475,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4" t="s">
         <v>286</v>
       </c>
-      <c r="C4" t="s">
-        <v>287</v>
-      </c>
       <c r="D4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -2498,28 +2504,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -2527,28 +2533,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -2556,28 +2562,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -2585,28 +2591,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>420</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -2614,28 +2620,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>420</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -2643,28 +2649,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
         <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -2672,28 +2678,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" t="s">
         <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" t="s">
-        <v>108</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -2701,28 +2707,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" t="s">
         <v>333</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>334</v>
-      </c>
-      <c r="D12" t="s">
-        <v>335</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -2730,28 +2736,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>420</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -2759,28 +2765,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>304</v>
+      </c>
+      <c r="C14" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" t="s">
         <v>305</v>
-      </c>
-      <c r="C14" t="s">
-        <v>307</v>
-      </c>
-      <c r="D14" t="s">
-        <v>306</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>419</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -2788,28 +2794,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>307</v>
+      </c>
+      <c r="C15" t="s">
+        <v>309</v>
+      </c>
+      <c r="D15" t="s">
         <v>308</v>
-      </c>
-      <c r="C15" t="s">
-        <v>310</v>
-      </c>
-      <c r="D15" t="s">
-        <v>309</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>101</v>
+        <v>419</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -2817,28 +2823,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -2846,28 +2852,28 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -2875,28 +2881,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>316</v>
+      </c>
+      <c r="C18" t="s">
         <v>317</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>318</v>
-      </c>
-      <c r="D18" t="s">
-        <v>319</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -2904,28 +2910,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -2933,28 +2939,28 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C20" t="s">
+        <v>363</v>
+      </c>
+      <c r="D20" t="s">
         <v>364</v>
-      </c>
-      <c r="D20" t="s">
-        <v>365</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -2962,28 +2968,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>369</v>
+      </c>
+      <c r="C21" t="s">
+        <v>363</v>
+      </c>
+      <c r="D21" t="s">
         <v>370</v>
-      </c>
-      <c r="C21" t="s">
-        <v>364</v>
-      </c>
-      <c r="D21" t="s">
-        <v>371</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G21" t="s">
         <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -2991,28 +2997,28 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -3020,28 +3026,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
       </c>
       <c r="H23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -3049,28 +3055,28 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
       </c>
       <c r="H24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3078,28 +3084,28 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
         <v>180</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>181</v>
-      </c>
-      <c r="D25" t="s">
-        <v>182</v>
       </c>
       <c r="E25" t="s">
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G25" t="s">
         <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -3107,28 +3113,28 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" t="s">
         <v>190</v>
       </c>
-      <c r="C26" t="s">
-        <v>191</v>
-      </c>
       <c r="D26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E26" t="s">
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G26" t="s">
         <v>24</v>
       </c>
       <c r="H26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -3136,28 +3142,28 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>254</v>
+      </c>
+      <c r="C27" t="s">
+        <v>265</v>
+      </c>
+      <c r="D27" t="s">
         <v>255</v>
-      </c>
-      <c r="C27" t="s">
-        <v>266</v>
-      </c>
-      <c r="D27" t="s">
-        <v>256</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
       </c>
       <c r="H27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -3165,28 +3171,28 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G28" t="s">
         <v>24</v>
       </c>
       <c r="H28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -3194,28 +3200,28 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>270</v>
+      </c>
+      <c r="C29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" t="s">
         <v>271</v>
-      </c>
-      <c r="C29" t="s">
-        <v>191</v>
-      </c>
-      <c r="D29" t="s">
-        <v>272</v>
       </c>
       <c r="E29" t="s">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
       </c>
       <c r="H29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -3223,28 +3229,28 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>277</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
         <v>278</v>
-      </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" t="s">
-        <v>279</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -3252,28 +3258,28 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" t="s">
         <v>181</v>
-      </c>
-      <c r="D31" t="s">
-        <v>182</v>
       </c>
       <c r="E31" t="s">
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G31" t="s">
         <v>24</v>
       </c>
       <c r="H31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -3281,28 +3287,28 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
       </c>
       <c r="H32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -3310,28 +3316,28 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>409</v>
+      </c>
+      <c r="C33" t="s">
         <v>410</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>411</v>
-      </c>
-      <c r="D33" t="s">
-        <v>412</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G33" t="s">
         <v>24</v>
       </c>
       <c r="H33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -3339,28 +3345,28 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34" t="s">
         <v>192</v>
-      </c>
-      <c r="C34" t="s">
-        <v>194</v>
-      </c>
-      <c r="D34" t="s">
-        <v>193</v>
       </c>
       <c r="E34" t="s">
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G34" t="s">
         <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -3368,28 +3374,28 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E35" t="s">
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
       </c>
       <c r="H35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -3397,28 +3403,28 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" t="s">
+        <v>219</v>
+      </c>
+      <c r="D36" t="s">
         <v>214</v>
-      </c>
-      <c r="C36" t="s">
-        <v>220</v>
-      </c>
-      <c r="D36" t="s">
-        <v>215</v>
       </c>
       <c r="E36" t="s">
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G36" t="s">
         <v>24</v>
       </c>
       <c r="H36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -3426,28 +3432,28 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>354</v>
+      </c>
+      <c r="C37" t="s">
         <v>355</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>356</v>
-      </c>
-      <c r="D37" t="s">
-        <v>357</v>
       </c>
       <c r="E37" t="s">
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G37" t="s">
         <v>24</v>
       </c>
       <c r="H37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -3455,28 +3461,28 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C38" t="s">
+        <v>221</v>
+      </c>
+      <c r="D38" t="s">
         <v>222</v>
-      </c>
-      <c r="D38" t="s">
-        <v>223</v>
       </c>
       <c r="E38" t="s">
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G38" t="s">
         <v>24</v>
       </c>
       <c r="H38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -3484,28 +3490,28 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>225</v>
+      </c>
+      <c r="C39" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" t="s">
         <v>226</v>
-      </c>
-      <c r="C39" t="s">
-        <v>228</v>
-      </c>
-      <c r="D39" t="s">
-        <v>227</v>
       </c>
       <c r="E39" t="s">
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
       </c>
       <c r="H39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -3513,28 +3519,28 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" t="s">
         <v>163</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>164</v>
-      </c>
-      <c r="D40" t="s">
-        <v>165</v>
       </c>
       <c r="E40" t="s">
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G40" t="s">
         <v>24</v>
       </c>
       <c r="H40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -3542,28 +3548,28 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" t="s">
         <v>210</v>
-      </c>
-      <c r="C41" t="s">
-        <v>213</v>
-      </c>
-      <c r="D41" t="s">
-        <v>211</v>
       </c>
       <c r="E41" t="s">
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G41" t="s">
         <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -3571,25 +3577,25 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" t="s">
+        <v>250</v>
+      </c>
+      <c r="D42" t="s">
         <v>236</v>
-      </c>
-      <c r="C42" t="s">
-        <v>251</v>
-      </c>
-      <c r="D42" t="s">
-        <v>237</v>
       </c>
       <c r="E42" t="s">
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -3597,28 +3603,28 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>385</v>
+      </c>
+      <c r="C43" t="s">
         <v>386</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>387</v>
-      </c>
-      <c r="D43" t="s">
-        <v>388</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G43" t="s">
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I43" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -3626,28 +3632,28 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>395</v>
+      </c>
+      <c r="C44" t="s">
+        <v>397</v>
+      </c>
+      <c r="D44" t="s">
         <v>396</v>
-      </c>
-      <c r="C44" t="s">
-        <v>398</v>
-      </c>
-      <c r="D44" t="s">
-        <v>397</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G44" t="s">
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I44" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3655,28 +3661,28 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>401</v>
+      </c>
+      <c r="C45" t="s">
         <v>402</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>403</v>
-      </c>
-      <c r="D45" t="s">
-        <v>404</v>
       </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G45" t="s">
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -3724,112 +3730,112 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" t="s">
         <v>384</v>
       </c>
-      <c r="J1" t="s">
-        <v>385</v>
-      </c>
       <c r="K1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L1" t="s">
+        <v>399</v>
+      </c>
+      <c r="M1" t="s">
+        <v>398</v>
+      </c>
+      <c r="N1" t="s">
         <v>400</v>
-      </c>
-      <c r="M1" t="s">
-        <v>399</v>
-      </c>
-      <c r="N1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
         <v>390</v>
       </c>
-      <c r="H2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>391</v>
       </c>
-      <c r="J2" t="s">
-        <v>392</v>
-      </c>
       <c r="K2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" t="s">
         <v>396</v>
       </c>
-      <c r="B3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C3" t="s">
-        <v>421</v>
-      </c>
-      <c r="D3" t="s">
-        <v>397</v>
-      </c>
       <c r="K3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F4" t="s">
         <v>404</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>405</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" t="s">
+        <v>408</v>
+      </c>
+      <c r="M4" t="s">
         <v>407</v>
-      </c>
-      <c r="L4" t="s">
-        <v>409</v>
-      </c>
-      <c r="M4" t="s">
-        <v>408</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -3878,8 +3884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3906,6 +3912,7 @@
     <col min="20" max="20" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="41.7265625" customWidth="1"/>
     <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="12.7265625" bestFit="1" customWidth="1"/>
@@ -3930,195 +3937,195 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>76</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>77</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>78</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>79</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>80</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>81</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>83</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>84</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>85</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>86</v>
       </c>
-      <c r="U1" t="s">
-        <v>87</v>
-      </c>
       <c r="V1" t="s">
+        <v>109</v>
+      </c>
+      <c r="W1" t="s">
         <v>110</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>111</v>
       </c>
-      <c r="X1" t="s">
-        <v>112</v>
-      </c>
       <c r="Y1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" t="s">
-        <v>57</v>
-      </c>
       <c r="AA1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB1" t="s">
         <v>115</v>
       </c>
-      <c r="AB1" t="s">
-        <v>116</v>
-      </c>
       <c r="AC1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AE1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF1" t="s">
         <v>121</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>122</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>123</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>124</v>
       </c>
-      <c r="AI1" t="s">
-        <v>125</v>
-      </c>
       <c r="AJ1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AK1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL1" t="s">
         <v>311</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>312</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>313</v>
       </c>
-      <c r="AN1" t="s">
-        <v>314</v>
-      </c>
       <c r="AO1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AP1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>336</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>337</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>338</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>339</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>340</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>341</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>342</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>343</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>421</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
       <c r="F2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>89</v>
       </c>
-      <c r="H2" t="s">
-        <v>90</v>
-      </c>
       <c r="I2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
         <v>92</v>
       </c>
-      <c r="J2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>423</v>
+      </c>
+      <c r="M2" t="s">
+        <v>424</v>
+      </c>
+      <c r="N2" t="s">
         <v>93</v>
       </c>
-      <c r="L2" t="s">
-        <v>424</v>
-      </c>
-      <c r="M2" t="s">
-        <v>425</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>426</v>
+      </c>
+      <c r="P2" t="s">
         <v>94</v>
       </c>
-      <c r="O2" t="s">
-        <v>427</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" t="s">
         <v>96</v>
-      </c>
-      <c r="R2" t="s">
-        <v>97</v>
       </c>
       <c r="S2">
         <v>98765438</v>
@@ -4127,63 +4134,66 @@
         <v>211</v>
       </c>
       <c r="U2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB2" t="s">
-        <v>426</v>
+        <v>425</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>89</v>
       </c>
-      <c r="H3" t="s">
-        <v>90</v>
-      </c>
       <c r="I3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
         <v>92</v>
       </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>423</v>
+      </c>
+      <c r="M3" t="s">
+        <v>424</v>
+      </c>
+      <c r="N3" t="s">
         <v>93</v>
       </c>
-      <c r="L3" t="s">
-        <v>424</v>
-      </c>
-      <c r="M3" t="s">
-        <v>425</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
+        <v>426</v>
+      </c>
+      <c r="P3" t="s">
         <v>94</v>
       </c>
-      <c r="O3" t="s">
-        <v>427</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="Q3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" t="s">
         <v>96</v>
-      </c>
-      <c r="R3" t="s">
-        <v>97</v>
       </c>
       <c r="S3">
         <v>98765438</v>
@@ -4192,10 +4202,10 @@
         <v>211</v>
       </c>
       <c r="U3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W3">
         <v>234</v>
@@ -4210,84 +4220,84 @@
         <v>1</v>
       </c>
       <c r="AA3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AC3">
         <v>45</v>
       </c>
       <c r="AD3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AF3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AG3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AH3">
         <v>54333</v>
       </c>
       <c r="AI3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
         <v>89</v>
       </c>
-      <c r="H4" t="s">
-        <v>90</v>
-      </c>
       <c r="I4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
         <v>92</v>
       </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>430</v>
+      </c>
+      <c r="M4" t="s">
+        <v>424</v>
+      </c>
+      <c r="N4" t="s">
         <v>93</v>
       </c>
-      <c r="L4" t="s">
-        <v>431</v>
-      </c>
-      <c r="M4" t="s">
-        <v>425</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
+        <v>426</v>
+      </c>
+      <c r="P4" t="s">
         <v>94</v>
       </c>
-      <c r="O4" t="s">
-        <v>427</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" t="s">
         <v>96</v>
-      </c>
-      <c r="R4" t="s">
-        <v>97</v>
       </c>
       <c r="S4">
         <v>98765438</v>
@@ -4296,10 +4306,10 @@
         <v>211</v>
       </c>
       <c r="U4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="W4">
         <v>234</v>
@@ -4314,124 +4324,124 @@
         <v>1</v>
       </c>
       <c r="AA4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AC4">
         <v>45</v>
       </c>
       <c r="AD4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AF4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AG4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AH4">
         <v>54333</v>
       </c>
       <c r="AI4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" t="s">
         <v>305</v>
       </c>
-      <c r="B5" t="s">
-        <v>304</v>
-      </c>
-      <c r="C5" t="s">
-        <v>421</v>
-      </c>
-      <c r="D5" t="s">
-        <v>306</v>
-      </c>
       <c r="F5" t="s">
+        <v>431</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>432</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" t="s">
         <v>308</v>
       </c>
-      <c r="B6" t="s">
-        <v>304</v>
-      </c>
-      <c r="C6" t="s">
-        <v>421</v>
-      </c>
-      <c r="D6" t="s">
-        <v>309</v>
-      </c>
       <c r="F6" t="s">
+        <v>431</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>432</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D7" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" t="s">
         <v>320</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s">
         <v>321</v>
       </c>
-      <c r="G7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" t="s">
-        <v>90</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M7" t="s">
+        <v>424</v>
+      </c>
+      <c r="N7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O7" t="s">
+        <v>426</v>
+      </c>
+      <c r="P7" t="s">
         <v>322</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" t="s">
-        <v>93</v>
-      </c>
-      <c r="L7" t="s">
-        <v>120</v>
-      </c>
-      <c r="M7" t="s">
-        <v>425</v>
-      </c>
-      <c r="N7" t="s">
-        <v>94</v>
-      </c>
-      <c r="O7" t="s">
-        <v>427</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="Q7" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="R7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S7">
         <v>98765438</v>
@@ -4440,10 +4450,10 @@
         <v>211</v>
       </c>
       <c r="U7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="W7">
         <v>234</v>
@@ -4458,177 +4468,177 @@
         <v>1</v>
       </c>
       <c r="AA7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AC7">
         <v>101</v>
       </c>
       <c r="AD7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AG7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AH7">
         <v>54333</v>
       </c>
       <c r="AI7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AJ8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AJ9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AK9">
         <v>23.33</v>
       </c>
       <c r="AL9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AM9">
         <v>2018</v>
       </c>
       <c r="AN9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AO10" t="s">
+        <v>349</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>344</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>345</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>423</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>346</v>
+      </c>
+      <c r="AT10" t="s">
         <v>350</v>
       </c>
-      <c r="AP10" t="s">
-        <v>345</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>346</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>424</v>
-      </c>
-      <c r="AS10" t="s">
+      <c r="AU10" t="s">
         <v>347</v>
       </c>
-      <c r="AT10" t="s">
+      <c r="AV10" t="s">
         <v>351</v>
       </c>
-      <c r="AU10" t="s">
-        <v>348</v>
-      </c>
-      <c r="AV10" t="s">
+      <c r="AW10" t="s">
         <v>352</v>
       </c>
-      <c r="AW10" t="s">
+      <c r="AX10" t="s">
         <v>353</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D11" t="s">
+        <v>367</v>
+      </c>
+      <c r="F11" t="s">
         <v>368</v>
       </c>
-      <c r="F11" t="s">
-        <v>369</v>
-      </c>
       <c r="G11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
         <v>89</v>
       </c>
-      <c r="H11" t="s">
-        <v>90</v>
-      </c>
       <c r="I11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
         <v>92</v>
       </c>
-      <c r="J11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
+        <v>119</v>
+      </c>
+      <c r="M11" t="s">
+        <v>424</v>
+      </c>
+      <c r="N11" t="s">
         <v>93</v>
       </c>
-      <c r="L11" t="s">
-        <v>120</v>
-      </c>
-      <c r="M11" t="s">
-        <v>425</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
+        <v>426</v>
+      </c>
+      <c r="P11" t="s">
         <v>94</v>
       </c>
-      <c r="O11" t="s">
-        <v>427</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="Q11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" t="s">
         <v>96</v>
-      </c>
-      <c r="R11" t="s">
-        <v>97</v>
       </c>
       <c r="S11">
         <v>98765438</v>
@@ -4637,10 +4647,10 @@
         <v>211</v>
       </c>
       <c r="U11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W11">
         <v>234</v>
@@ -4655,100 +4665,100 @@
         <v>1</v>
       </c>
       <c r="AA11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AC11">
         <v>45</v>
       </c>
       <c r="AD11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AG11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AH11">
         <v>54333</v>
       </c>
       <c r="AI11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>366</v>
+      </c>
+      <c r="B12" t="s">
+        <v>365</v>
+      </c>
+      <c r="C12" t="s">
+        <v>420</v>
+      </c>
+      <c r="D12" t="s">
         <v>367</v>
       </c>
-      <c r="B12" t="s">
-        <v>366</v>
-      </c>
-      <c r="C12" t="s">
-        <v>421</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>372</v>
+      </c>
+      <c r="F12" t="s">
         <v>368</v>
-      </c>
-      <c r="E12" t="s">
-        <v>373</v>
-      </c>
-      <c r="F12" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>369</v>
+      </c>
+      <c r="B13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C13" t="s">
+        <v>420</v>
+      </c>
+      <c r="D13" t="s">
         <v>370</v>
       </c>
-      <c r="B13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C13" t="s">
-        <v>421</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>371</v>
-      </c>
-      <c r="E13" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B14" t="s">
+        <v>376</v>
+      </c>
+      <c r="C14" t="s">
+        <v>420</v>
+      </c>
+      <c r="D14" t="s">
+        <v>375</v>
+      </c>
+      <c r="F14" t="s">
         <v>377</v>
       </c>
-      <c r="B14" t="s">
-        <v>377</v>
-      </c>
-      <c r="C14" t="s">
-        <v>421</v>
-      </c>
-      <c r="D14" t="s">
-        <v>376</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="AJ14" t="s">
         <v>378</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>379</v>
       </c>
       <c r="AK14">
         <v>345</v>
       </c>
       <c r="AL14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AM14">
         <v>2020</v>
       </c>
       <c r="AN14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4799,57 +4809,57 @@
         <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
       <c r="O1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
         <v>421</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" t="s">
-        <v>422</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -4858,39 +4868,39 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2">
         <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F3" t="s">
         <v>295</v>
       </c>
-      <c r="F3" t="s">
-        <v>296</v>
-      </c>
       <c r="G3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -4899,39 +4909,39 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K3">
         <v>111</v>
       </c>
       <c r="L3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" t="s">
         <v>298</v>
       </c>
-      <c r="B4" t="s">
-        <v>299</v>
-      </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -4978,51 +4988,51 @@
         <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" t="s">
         <v>239</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>240</v>
       </c>
-      <c r="H1" t="s">
-        <v>241</v>
-      </c>
       <c r="I1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" t="s">
         <v>245</v>
       </c>
-      <c r="K1" t="s">
-        <v>246</v>
-      </c>
       <c r="L1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M1" t="s">
         <v>248</v>
-      </c>
-      <c r="M1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" t="s">
         <v>236</v>
-      </c>
-      <c r="B2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="E2" t="s">
-        <v>237</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5031,22 +5041,22 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L2">
         <v>122</v>
       </c>
       <c r="M2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -5114,129 +5124,129 @@
         <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>131</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>132</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>133</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>134</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>135</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>136</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>137</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>138</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>139</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>140</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>141</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>142</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>143</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>144</v>
       </c>
-      <c r="Y1" t="s">
-        <v>145</v>
-      </c>
       <c r="Z1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AA1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB1" t="s">
         <v>186</v>
       </c>
-      <c r="AB1" t="s">
-        <v>187</v>
-      </c>
       <c r="AC1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AD1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AE1" t="s">
         <v>259</v>
       </c>
-      <c r="AE1" t="s">
-        <v>260</v>
-      </c>
       <c r="AF1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AG1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
         <v>150</v>
       </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>151</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>152</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>153</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>154</v>
       </c>
-      <c r="L2" t="s">
-        <v>155</v>
-      </c>
       <c r="M2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N2">
         <v>2019</v>
@@ -5245,297 +5255,297 @@
         <v>2019</v>
       </c>
       <c r="P2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q2" t="s">
         <v>156</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
+        <v>232</v>
+      </c>
+      <c r="S2" t="s">
         <v>157</v>
       </c>
-      <c r="R2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>158</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>159</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>160</v>
-      </c>
-      <c r="W2" t="s">
-        <v>161</v>
       </c>
       <c r="X2">
         <v>2019</v>
       </c>
       <c r="Y2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H3" t="s">
-        <v>167</v>
-      </c>
       <c r="K3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O3">
         <v>2020</v>
       </c>
       <c r="Z3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" t="s">
         <v>184</v>
       </c>
-      <c r="E4" t="s">
-        <v>185</v>
-      </c>
       <c r="K4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA4" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB4" t="s">
         <v>188</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" t="s">
         <v>184</v>
       </c>
-      <c r="E5" t="s">
-        <v>185</v>
-      </c>
       <c r="F5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" t="s">
         <v>255</v>
       </c>
-      <c r="B6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G6" t="s">
+        <v>266</v>
+      </c>
+      <c r="K6" t="s">
+        <v>153</v>
+      </c>
+      <c r="S6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>257</v>
+      </c>
+      <c r="AD6" t="s">
         <v>256</v>
       </c>
-      <c r="E6" t="s">
-        <v>264</v>
-      </c>
-      <c r="G6" t="s">
-        <v>267</v>
-      </c>
-      <c r="K6" t="s">
-        <v>154</v>
-      </c>
-      <c r="S6" t="s">
-        <v>158</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>258</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>257</v>
-      </c>
       <c r="AE6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AF6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E7" t="s">
         <v>272</v>
       </c>
-      <c r="E7" t="s">
-        <v>273</v>
-      </c>
       <c r="K7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AB7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D8" t="s">
         <v>271</v>
       </c>
-      <c r="B8" t="s">
-        <v>270</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>272</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>273</v>
       </c>
-      <c r="F8" t="s">
-        <v>274</v>
-      </c>
       <c r="K8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AA8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" t="s">
         <v>278</v>
       </c>
-      <c r="B9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>279</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>280</v>
       </c>
-      <c r="F9" t="s">
+      <c r="K9" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA9" t="s">
         <v>281</v>
       </c>
-      <c r="K9" t="s">
-        <v>277</v>
-      </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>282</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA10" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB10" t="s">
         <v>188</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
@@ -5599,7 +5609,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -5607,16 +5617,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -5659,78 +5669,78 @@
         <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" t="s">
         <v>224</v>
-      </c>
-      <c r="B3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" t="s">
-        <v>421</v>
-      </c>
-      <c r="D3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F3" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D4" t="s">
         <v>226</v>
       </c>
-      <c r="B4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" t="s">
-        <v>421</v>
-      </c>
-      <c r="D4" t="s">
-        <v>227</v>
-      </c>
       <c r="F4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" t="s">
         <v>229</v>
       </c>
-      <c r="B5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" t="s">
-        <v>421</v>
-      </c>
-      <c r="D5" t="s">
-        <v>230</v>
-      </c>
       <c r="F5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed xpath for viewproject and made code changes.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3173F74D-8188-4CE0-9931-67BE399CB39B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8434B6B7-85AD-4361-AB66-FC9641957843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -2632,7 +2632,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>419</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -4779,8 +4779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
comiting the test dat
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF804471-0660-4EB8-8AD2-8063E1E004B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4165C5-C2F5-4E02-8840-F0E73871B38C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21435" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21480" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1366,7 +1366,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1394,6 +1394,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1441,7 +1448,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1449,6 +1456,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1790,7 +1798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2635,7 +2643,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>419</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -3575,29 +3583,29 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F42" t="s">
         <v>419</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="7" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made changes in testdata and object repositories
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahid\git\ProdLatestDis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4165C5-C2F5-4E02-8840-F0E73871B38C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86989AE7-024F-41D7-8EAF-7392D0E0ED17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21480" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="440">
   <si>
     <t>Environment</t>
   </si>
@@ -1360,6 +1360,15 @@
   </si>
   <si>
     <t>Muthukuru, Shamant (smuthukuru@usaid.gov)</t>
+  </si>
+  <si>
+    <t>Ponnuru, Sri (sponnuru@usaid.gov)</t>
+  </si>
+  <si>
+    <t>Higuera, Alfredo (ahiguera@usaid.gov)</t>
+  </si>
+  <si>
+    <t>Office name 10/5</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2383,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2788,7 +2797,7 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>419</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -2817,7 +2826,7 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>419</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -2846,7 +2855,7 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>419</v>
+        <v>100</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
@@ -2875,7 +2884,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>419</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -3895,8 +3904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AR2" sqref="AR2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3906,13 +3915,13 @@
     <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.7265625" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
     <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.7265625" customWidth="1"/>
     <col min="13" max="13" width="36.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.81640625" bestFit="1" customWidth="1"/>
@@ -4434,10 +4443,10 @@
         <v>92</v>
       </c>
       <c r="L7" t="s">
-        <v>119</v>
+        <v>439</v>
       </c>
       <c r="M7" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="N7" t="s">
         <v>93</v>
@@ -4482,7 +4491,7 @@
         <v>116</v>
       </c>
       <c r="AB7" t="s">
-        <v>232</v>
+        <v>438</v>
       </c>
       <c r="AC7">
         <v>101</v>
@@ -4504,6 +4513,9 @@
       </c>
       <c r="AI7" t="s">
         <v>233</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.35">
@@ -4535,6 +4547,9 @@
       </c>
       <c r="D9" t="s">
         <v>319</v>
+      </c>
+      <c r="F9" t="s">
+        <v>429</v>
       </c>
       <c r="AJ9" t="s">
         <v>300</v>

</xml_diff>